<commit_message>
Speed up, different solution initialization.
</commit_message>
<xml_diff>
--- a/algorithms/results/comparison.xlsx
+++ b/algorithms/results/comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\akcijanje\nauka\moji radovi\aktivno\k-domination\algorithms\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC75203-63EF-4D08-881C-30E9DEBF22F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631388B2-D301-451E-B675-7E49472B5FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3555" windowWidth="29040" windowHeight="15840" xr2:uid="{9811A06C-B274-406A-BE4D-18F0FA4A89B1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="34">
   <si>
     <t>bath.txt</t>
   </si>
@@ -501,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C114BA-E20E-4760-908C-9E2FAA6D010C}">
-  <dimension ref="A1:K74"/>
+  <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:Q1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="M62" sqref="M62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +514,7 @@
     <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>21</v>
@@ -528,8 +528,17 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1">
+        <v>150</v>
+      </c>
+      <c r="Q1">
+        <v>631.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>27</v>
@@ -547,8 +556,17 @@
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>182</v>
+      </c>
+      <c r="Q2">
+        <v>3637.73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -582,8 +600,17 @@
       <c r="K3" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>89</v>
+      </c>
+      <c r="Q3">
+        <v>714.64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -619,8 +646,17 @@
         <f>IF($B4=I4, "opt", "")</f>
         <v/>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>165</v>
+      </c>
+      <c r="Q4">
+        <v>3447.42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -656,8 +692,17 @@
         <f t="shared" ref="K5:K23" si="1">IF($B5=I5, "opt", "")</f>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <v>168</v>
+      </c>
+      <c r="Q5">
+        <v>1174.47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -693,8 +738,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6">
+        <v>162</v>
+      </c>
+      <c r="Q6">
+        <v>1435.66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -730,8 +784,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7">
+        <v>169</v>
+      </c>
+      <c r="Q7">
+        <v>1391.51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -767,8 +830,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>7</v>
+      </c>
+      <c r="P8">
+        <v>190</v>
+      </c>
+      <c r="Q8">
+        <v>1329.91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -804,8 +876,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>8</v>
+      </c>
+      <c r="P9">
+        <v>166</v>
+      </c>
+      <c r="Q9">
+        <v>3240.09</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -841,8 +922,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O10" t="s">
+        <v>9</v>
+      </c>
+      <c r="P10">
+        <v>162</v>
+      </c>
+      <c r="Q10">
+        <v>3571.87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -878,8 +968,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O11" t="s">
+        <v>10</v>
+      </c>
+      <c r="P11">
+        <v>125</v>
+      </c>
+      <c r="Q11">
+        <v>2636.94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -915,8 +1014,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O12" t="s">
+        <v>11</v>
+      </c>
+      <c r="P12">
+        <v>214</v>
+      </c>
+      <c r="Q12">
+        <v>5236.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -952,8 +1060,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>12</v>
+      </c>
+      <c r="P13">
+        <v>166</v>
+      </c>
+      <c r="Q13">
+        <v>1399.34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -989,8 +1106,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O14" t="s">
+        <v>13</v>
+      </c>
+      <c r="P14">
+        <v>191</v>
+      </c>
+      <c r="Q14">
+        <v>3558.47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1026,8 +1152,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O15" t="s">
+        <v>14</v>
+      </c>
+      <c r="P15">
+        <v>93</v>
+      </c>
+      <c r="Q15">
+        <v>2570.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1063,8 +1198,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>15</v>
+      </c>
+      <c r="P16">
+        <v>128</v>
+      </c>
+      <c r="Q16">
+        <v>2018.32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1100,8 +1244,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>16</v>
+      </c>
+      <c r="P17">
+        <v>180</v>
+      </c>
+      <c r="Q17">
+        <v>2915.07</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1137,8 +1290,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>17</v>
+      </c>
+      <c r="P18">
+        <v>104</v>
+      </c>
+      <c r="Q18">
+        <v>891.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1174,8 +1336,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O19" t="s">
+        <v>18</v>
+      </c>
+      <c r="P19">
+        <v>151</v>
+      </c>
+      <c r="Q19">
+        <v>1895.86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1211,8 +1382,17 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O20" t="s">
+        <v>19</v>
+      </c>
+      <c r="P20">
+        <v>142</v>
+      </c>
+      <c r="Q20">
+        <v>1693.27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1249,7 +1429,7 @@
         <v>opt</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1286,7 +1466,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1323,7 +1503,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1367,8 +1547,11 @@
         <f>COUNTIF(K4:K23, "opt")</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
         <v>31</v>
@@ -1383,7 +1566,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
         <v>27</v>
@@ -1402,7 +1585,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
@@ -1437,7 +1620,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1474,7 +1657,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1511,7 +1694,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1548,7 +1731,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -2177,7 +2360,7 @@
         <v>opt</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>30</v>
       </c>
@@ -2221,8 +2404,11 @@
         <f>COUNTIF(K29:K48, "opt")</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2" t="s">
         <v>33</v>
@@ -2237,7 +2423,7 @@
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2" t="s">
         <v>27</v>
@@ -2256,7 +2442,7 @@
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>20</v>
       </c>
@@ -2291,7 +2477,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -2307,6 +2493,12 @@
       <c r="E54">
         <v>3608.26</v>
       </c>
+      <c r="F54">
+        <v>150</v>
+      </c>
+      <c r="G54">
+        <v>631.5</v>
+      </c>
       <c r="H54" t="str">
         <f>IF($B54=F54, "opt", "")</f>
         <v/>
@@ -2322,7 +2514,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1</v>
       </c>
@@ -2338,6 +2530,12 @@
       <c r="E55">
         <v>1985.8</v>
       </c>
+      <c r="F55">
+        <v>182</v>
+      </c>
+      <c r="G55">
+        <v>3637.73</v>
+      </c>
       <c r="H55" t="str">
         <f t="shared" ref="H55:H73" si="14">IF($B55=F55, "opt", "")</f>
         <v/>
@@ -2353,7 +2551,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -2369,6 +2567,12 @@
       <c r="E56">
         <v>179.16</v>
       </c>
+      <c r="F56">
+        <v>89</v>
+      </c>
+      <c r="G56">
+        <v>714.64</v>
+      </c>
       <c r="H56" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2384,7 +2588,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>3</v>
       </c>
@@ -2400,6 +2604,12 @@
       <c r="E57">
         <v>3631.76</v>
       </c>
+      <c r="F57">
+        <v>165</v>
+      </c>
+      <c r="G57">
+        <v>3447.42</v>
+      </c>
       <c r="H57" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2415,7 +2625,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -2431,6 +2641,12 @@
       <c r="E58">
         <v>911.98</v>
       </c>
+      <c r="F58">
+        <v>168</v>
+      </c>
+      <c r="G58">
+        <v>1174.47</v>
+      </c>
       <c r="H58" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2446,7 +2662,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -2462,6 +2678,12 @@
       <c r="E59">
         <v>3604.64</v>
       </c>
+      <c r="F59">
+        <v>162</v>
+      </c>
+      <c r="G59">
+        <v>1435.66</v>
+      </c>
       <c r="H59" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2477,7 +2699,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -2493,6 +2715,12 @@
       <c r="E60">
         <v>3655.54</v>
       </c>
+      <c r="F60">
+        <v>169</v>
+      </c>
+      <c r="G60">
+        <v>1391.51</v>
+      </c>
       <c r="H60" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2508,7 +2736,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -2524,6 +2752,12 @@
       <c r="E61">
         <v>3648.06</v>
       </c>
+      <c r="F61">
+        <v>190</v>
+      </c>
+      <c r="G61">
+        <v>1329.91</v>
+      </c>
       <c r="H61" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2539,7 +2773,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -2555,6 +2789,12 @@
       <c r="E62">
         <v>329.38</v>
       </c>
+      <c r="F62">
+        <v>166</v>
+      </c>
+      <c r="G62">
+        <v>3240.09</v>
+      </c>
       <c r="H62" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2570,7 +2810,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>9</v>
       </c>
@@ -2586,6 +2826,12 @@
       <c r="E63">
         <v>3602.38</v>
       </c>
+      <c r="F63">
+        <v>162</v>
+      </c>
+      <c r="G63">
+        <v>3571.87</v>
+      </c>
       <c r="H63" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2601,7 +2847,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -2616,6 +2862,12 @@
       </c>
       <c r="E64">
         <v>338.36</v>
+      </c>
+      <c r="F64">
+        <v>125</v>
+      </c>
+      <c r="G64">
+        <v>2636.94</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="14"/>
@@ -2648,6 +2900,12 @@
       <c r="E65">
         <v>3620.36</v>
       </c>
+      <c r="F65">
+        <v>214</v>
+      </c>
+      <c r="G65">
+        <v>5236.25</v>
+      </c>
       <c r="H65" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2679,6 +2937,12 @@
       <c r="E66">
         <v>913.1</v>
       </c>
+      <c r="F66">
+        <v>166</v>
+      </c>
+      <c r="G66">
+        <v>1399.34</v>
+      </c>
       <c r="H66" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2710,6 +2974,12 @@
       <c r="E67">
         <v>236.64</v>
       </c>
+      <c r="F67">
+        <v>191</v>
+      </c>
+      <c r="G67">
+        <v>3558.47</v>
+      </c>
       <c r="H67" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2741,6 +3011,12 @@
       <c r="E68">
         <v>17.079999999999998</v>
       </c>
+      <c r="F68">
+        <v>93</v>
+      </c>
+      <c r="G68">
+        <v>2570.6</v>
+      </c>
       <c r="H68" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2772,6 +3048,12 @@
       <c r="E69">
         <v>227.07</v>
       </c>
+      <c r="F69">
+        <v>128</v>
+      </c>
+      <c r="G69">
+        <v>2018.32</v>
+      </c>
       <c r="H69" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2803,6 +3085,12 @@
       <c r="E70">
         <v>3650.96</v>
       </c>
+      <c r="F70">
+        <v>180</v>
+      </c>
+      <c r="G70">
+        <v>2915.07</v>
+      </c>
       <c r="H70" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2834,6 +3122,12 @@
       <c r="E71">
         <v>53.23</v>
       </c>
+      <c r="F71">
+        <v>104</v>
+      </c>
+      <c r="G71">
+        <v>891.9</v>
+      </c>
       <c r="H71" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2865,6 +3159,12 @@
       <c r="E72">
         <v>3637.62</v>
       </c>
+      <c r="F72">
+        <v>151</v>
+      </c>
+      <c r="G72">
+        <v>1895.86</v>
+      </c>
       <c r="H72" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2896,6 +3196,12 @@
       <c r="E73">
         <v>31.71</v>
       </c>
+      <c r="F73">
+        <v>142</v>
+      </c>
+      <c r="G73">
+        <v>1693.27</v>
+      </c>
       <c r="H73" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -2931,13 +3237,13 @@
         <f t="shared" ref="E74" si="18">AVERAGE(E54:E73)</f>
         <v>1894.1545000000006</v>
       </c>
-      <c r="F74" s="1" t="e">
+      <c r="F74" s="1">
         <f t="shared" ref="F74" si="19">AVERAGE(F54:F73)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G74" s="1" t="e">
+        <v>154.85</v>
+      </c>
+      <c r="G74" s="1">
         <f t="shared" ref="G74" si="20">AVERAGE(G54:G73)</f>
-        <v>#DIV/0!</v>
+        <v>2269.5409999999997</v>
       </c>
       <c r="H74" s="1">
         <f>COUNTIF(H54:H73, "opt")</f>

</xml_diff>

<commit_message>
Results when d=(10, 40)
</commit_message>
<xml_diff>
--- a/algorithms/results/comparison.xlsx
+++ b/algorithms/results/comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\akcijanje\nauka\moji radovi\aktivno\k-domination\algorithms\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A0B681-BF33-436F-BBF0-8D10EBB52D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81291042-17B3-46D0-BFA2-9769AAE940A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3555" windowWidth="29040" windowHeight="15840" xr2:uid="{9811A06C-B274-406A-BE4D-18F0FA4A89B1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="36">
   <si>
     <t>bath.txt</t>
   </si>
@@ -140,7 +140,10 @@
     <t>k=4</t>
   </si>
   <si>
-    <t>VNS 14.1.2023. 23:35:20</t>
+    <t>VNS d(5_30) 14.1.2023. 23:35:20</t>
+  </si>
+  <si>
+    <t>VNS d(10_40) 14.1.2023. 23:35:20</t>
   </si>
 </sst>
 </file>
@@ -184,12 +187,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,20 +508,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C114BA-E20E-4760-908C-9E2FAA6D010C}">
-  <dimension ref="A1:Q74"/>
+  <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:S1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:V1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>21</v>
@@ -534,8 +541,11 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>27</v>
@@ -544,22 +554,27 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -602,8 +617,17 @@
       <c r="N3" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,7 +647,7 @@
         <v>38</v>
       </c>
       <c r="G4">
-        <v>317.54000000000002</v>
+        <v>865.69</v>
       </c>
       <c r="H4" t="str">
         <f>IF($B4=F4, "opt", "")</f>
@@ -633,25 +657,35 @@
         <v>38</v>
       </c>
       <c r="J4">
-        <v>535.66999999999996</v>
+        <v>317.54000000000002</v>
       </c>
       <c r="K4" t="str">
         <f>IF($B4=I4, "opt", "")</f>
         <v>opt</v>
       </c>
       <c r="L4">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M4">
-        <v>239.56</v>
+        <v>535.66999999999996</v>
       </c>
       <c r="N4" t="str">
         <f>IF($B4=L4, "opt", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+        <v>opt</v>
+      </c>
+      <c r="O4">
+        <v>39</v>
+      </c>
+      <c r="P4">
+        <v>239.56</v>
+      </c>
+      <c r="Q4" t="str">
+        <f>IF($B4=O4, "opt", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B5">
@@ -667,37 +701,47 @@
         <v>0.74</v>
       </c>
       <c r="F5">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5">
-        <v>102.76</v>
+        <v>443.57</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" ref="H5:H23" si="0">IF($B5=F5, "opt", "")</f>
-        <v/>
+        <v>opt</v>
       </c>
       <c r="I5">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J5">
-        <v>2996.25</v>
+        <v>102.76</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" ref="K5:K23" si="1">IF($B5=I5, "opt", "")</f>
         <v/>
       </c>
       <c r="L5">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M5">
-        <v>2857.14</v>
+        <v>2996.25</v>
       </c>
       <c r="N5" t="str">
         <f t="shared" ref="N5:N23" si="2">IF($B5=L5, "opt", "")</f>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>44</v>
+      </c>
+      <c r="P5">
+        <v>2857.14</v>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" ref="Q5:Q23" si="3">IF($B5=O5, "opt", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -717,35 +761,45 @@
         <v>21</v>
       </c>
       <c r="G6">
-        <v>103.26</v>
+        <v>31.04</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
         <v>opt</v>
       </c>
       <c r="I6">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J6">
-        <v>698.58</v>
+        <v>103.26</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>opt</v>
       </c>
       <c r="L6">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M6">
-        <v>425.46</v>
+        <v>698.58</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="O6">
+        <v>23</v>
+      </c>
+      <c r="P6">
+        <v>425.46</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B7">
@@ -761,37 +815,47 @@
         <v>0.49</v>
       </c>
       <c r="F7">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7">
-        <v>10.23</v>
+        <v>377.94</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>opt</v>
       </c>
       <c r="I7">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J7">
-        <v>2024.36</v>
+        <v>10.23</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L7">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M7">
-        <v>1488.4</v>
+        <v>2024.36</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>41</v>
+      </c>
+      <c r="P7">
+        <v>1488.4</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -811,7 +875,7 @@
         <v>39</v>
       </c>
       <c r="G8">
-        <v>14.55</v>
+        <v>1589.66</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -821,25 +885,35 @@
         <v>39</v>
       </c>
       <c r="J8">
-        <v>1765.89</v>
+        <v>14.55</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="1"/>
         <v>opt</v>
       </c>
       <c r="L8">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M8">
-        <v>2772.73</v>
+        <v>1765.89</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+        <v>opt</v>
+      </c>
+      <c r="O8">
+        <v>40</v>
+      </c>
+      <c r="P8">
+        <v>2772.73</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B9">
@@ -858,7 +932,7 @@
         <v>38</v>
       </c>
       <c r="G9">
-        <v>1179.68</v>
+        <v>802.97</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -868,24 +942,34 @@
         <v>38</v>
       </c>
       <c r="J9">
-        <v>2113.4499999999998</v>
+        <v>1179.68</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
         <v>opt</v>
       </c>
       <c r="L9">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M9">
-        <v>1158.5</v>
+        <v>2113.4499999999998</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>opt</v>
+      </c>
+      <c r="O9">
+        <v>39</v>
+      </c>
+      <c r="P9">
+        <v>1158.5</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -905,35 +989,45 @@
         <v>38</v>
       </c>
       <c r="G10">
-        <v>1782.11</v>
+        <v>221.94</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
         <v>opt</v>
       </c>
       <c r="I10">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J10">
-        <v>863.68</v>
+        <v>1782.11</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>opt</v>
       </c>
       <c r="L10">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="M10">
-        <v>292.3</v>
+        <v>863.68</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="O10">
+        <v>44</v>
+      </c>
+      <c r="P10">
+        <v>292.3</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B11">
@@ -952,35 +1046,45 @@
         <v>50</v>
       </c>
       <c r="G11">
-        <v>24.48</v>
+        <v>348.19</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
         <v>opt</v>
       </c>
       <c r="I11">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J11">
-        <v>855.99</v>
+        <v>24.48</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>opt</v>
       </c>
       <c r="L11">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M11">
-        <v>614.62</v>
+        <v>855.99</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="O11">
+        <v>51</v>
+      </c>
+      <c r="P11">
+        <v>614.62</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12">
@@ -996,38 +1100,48 @@
         <v>0.47</v>
       </c>
       <c r="F12">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G12">
-        <v>131.19</v>
+        <v>849.36</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>opt</v>
       </c>
       <c r="I12">
         <v>42</v>
       </c>
       <c r="J12">
-        <v>2885.75</v>
+        <v>131.19</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L12">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M12">
-        <v>3123.37</v>
+        <v>2885.75</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="O12">
+        <v>44</v>
+      </c>
+      <c r="P12">
+        <v>3123.37</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B13">
@@ -1046,7 +1160,7 @@
         <v>39</v>
       </c>
       <c r="G13">
-        <v>1451.66</v>
+        <v>646.91999999999996</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -1056,25 +1170,35 @@
         <v>39</v>
       </c>
       <c r="J13">
-        <v>2981.75</v>
+        <v>1451.66</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L13">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M13">
-        <v>1896.54</v>
+        <v>2981.75</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="O13">
+        <v>41</v>
+      </c>
+      <c r="P13">
+        <v>1896.54</v>
+      </c>
+      <c r="Q13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B14">
@@ -1093,35 +1217,45 @@
         <v>29</v>
       </c>
       <c r="G14">
-        <v>88.49</v>
+        <v>190.4</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I14">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J14">
-        <v>1720.72</v>
+        <v>88.49</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L14">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M14">
-        <v>3563.82</v>
+        <v>1720.72</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="O14">
+        <v>32</v>
+      </c>
+      <c r="P14">
+        <v>3563.82</v>
+      </c>
+      <c r="Q14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B15">
@@ -1137,38 +1271,48 @@
         <v>0.63</v>
       </c>
       <c r="F15">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15">
-        <v>354.86</v>
+        <v>2763.95</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I15">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="J15">
-        <v>4064.85</v>
+        <v>354.86</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L15">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="M15">
-        <v>2013.71</v>
+        <v>4064.85</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="O15">
+        <v>45</v>
+      </c>
+      <c r="P15">
+        <v>2013.71</v>
+      </c>
+      <c r="Q15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B16">
@@ -1184,38 +1328,48 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="F16">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G16">
-        <v>1541.83</v>
+        <v>61.75</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
-        <v>opt</v>
+        <v/>
       </c>
       <c r="I16">
         <v>44</v>
       </c>
       <c r="J16">
-        <v>3410.89</v>
+        <v>1541.83</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="1"/>
         <v>opt</v>
       </c>
       <c r="L16">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M16">
-        <v>792.09</v>
+        <v>3410.89</v>
       </c>
       <c r="N16" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+        <v>opt</v>
+      </c>
+      <c r="O16">
+        <v>47</v>
+      </c>
+      <c r="P16">
+        <v>792.09</v>
+      </c>
+      <c r="Q16" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B17">
@@ -1234,35 +1388,45 @@
         <v>44</v>
       </c>
       <c r="G17">
-        <v>85.64</v>
+        <v>115</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
         <v>opt</v>
       </c>
       <c r="I17">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J17">
-        <v>3547.01</v>
+        <v>85.64</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>opt</v>
       </c>
       <c r="L17">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M17">
-        <v>3016.44</v>
+        <v>3547.01</v>
       </c>
       <c r="N17" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="O17">
+        <v>46</v>
+      </c>
+      <c r="P17">
+        <v>3016.44</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B18">
@@ -1281,35 +1445,45 @@
         <v>25</v>
       </c>
       <c r="G18">
-        <v>2.81</v>
+        <v>0.54</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I18">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J18">
-        <v>36.47</v>
+        <v>2.81</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="1"/>
-        <v>opt</v>
+        <v/>
       </c>
       <c r="L18">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M18">
-        <v>152.80000000000001</v>
+        <v>36.47</v>
       </c>
       <c r="N18" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+        <v>opt</v>
+      </c>
+      <c r="O18">
+        <v>25</v>
+      </c>
+      <c r="P18">
+        <v>152.80000000000001</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B19">
@@ -1328,7 +1502,7 @@
         <v>31</v>
       </c>
       <c r="G19">
-        <v>268.31</v>
+        <v>181.26</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -1338,24 +1512,34 @@
         <v>31</v>
       </c>
       <c r="J19">
-        <v>1203.18</v>
+        <v>268.31</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="1"/>
         <v>opt</v>
       </c>
       <c r="L19">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="M19">
-        <v>180.01</v>
+        <v>1203.18</v>
       </c>
       <c r="N19" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>opt</v>
+      </c>
+      <c r="O19">
+        <v>36</v>
+      </c>
+      <c r="P19">
+        <v>180.01</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -1375,35 +1559,45 @@
         <v>42</v>
       </c>
       <c r="G20">
-        <v>1663.5</v>
+        <v>1333.45</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
         <v>opt</v>
       </c>
       <c r="I20">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J20">
-        <v>2297.98</v>
+        <v>1663.5</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>opt</v>
       </c>
       <c r="L20">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M20">
-        <v>2892.3</v>
+        <v>2297.98</v>
       </c>
       <c r="N20" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="O20">
+        <v>46</v>
+      </c>
+      <c r="P20">
+        <v>2892.3</v>
+      </c>
+      <c r="Q20" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B21">
@@ -1422,7 +1616,7 @@
         <v>25</v>
       </c>
       <c r="G21">
-        <v>52.26</v>
+        <v>34.53</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -1432,7 +1626,7 @@
         <v>25</v>
       </c>
       <c r="J21">
-        <v>213.16</v>
+        <v>52.26</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="1"/>
@@ -1442,14 +1636,24 @@
         <v>25</v>
       </c>
       <c r="M21">
-        <v>472.69</v>
+        <v>213.16</v>
       </c>
       <c r="N21" t="str">
         <f t="shared" si="2"/>
         <v>opt</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <v>25</v>
+      </c>
+      <c r="P21">
+        <v>472.69</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" si="3"/>
+        <v>opt</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -1469,7 +1673,7 @@
         <v>36</v>
       </c>
       <c r="G22">
-        <v>194.11</v>
+        <v>558.71</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -1479,25 +1683,35 @@
         <v>36</v>
       </c>
       <c r="J22">
-        <v>1604.97</v>
+        <v>194.11</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="1"/>
         <v>opt</v>
       </c>
       <c r="L22">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M22">
-        <v>1303.21</v>
+        <v>1604.97</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+        <v>opt</v>
+      </c>
+      <c r="O22">
+        <v>37</v>
+      </c>
+      <c r="P22">
+        <v>1303.21</v>
+      </c>
+      <c r="Q22" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B23">
@@ -1516,7 +1730,7 @@
         <v>32</v>
       </c>
       <c r="G23">
-        <v>25.36</v>
+        <v>284.64</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -1526,24 +1740,34 @@
         <v>32</v>
       </c>
       <c r="J23">
-        <v>1358.42</v>
+        <v>25.36</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="1"/>
         <v>opt</v>
       </c>
       <c r="L23">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M23">
-        <v>403.23</v>
+        <v>1358.42</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>opt</v>
+      </c>
+      <c r="O23">
+        <v>33</v>
+      </c>
+      <c r="P23">
+        <v>403.23</v>
+      </c>
+      <c r="Q23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1552,58 +1776,70 @@
         <v>36.1</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" ref="C24:J24" si="3">AVERAGE(C4:C23)</f>
+        <f t="shared" ref="C24:M24" si="4">AVERAGE(C4:C23)</f>
         <v>36.1</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.37649999999999995</v>
       </c>
       <c r="F24" s="1">
-        <f>AVERAGE(F4:F23)</f>
-        <v>36.549999999999997</v>
+        <f t="shared" si="4"/>
+        <v>36.35</v>
       </c>
       <c r="G24" s="1">
-        <f>AVERAGE(G4:G23)</f>
-        <v>469.73150000000015</v>
+        <f t="shared" si="4"/>
+        <v>585.07549999999992</v>
       </c>
       <c r="H24" s="1">
         <f>COUNTIF(H4:H23, "opt")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" si="3"/>
-        <v>37.9</v>
+        <f>AVERAGE(I4:I23)</f>
+        <v>36.549999999999997</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="3"/>
-        <v>1858.9510000000005</v>
+        <f>AVERAGE(J4:J23)</f>
+        <v>469.73150000000015</v>
       </c>
       <c r="K24" s="1">
         <f>COUNTIF(K4:K23, "opt")</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="L24" s="1">
-        <f t="shared" ref="L24" si="4">AVERAGE(L4:L23)</f>
-        <v>38.9</v>
+        <f t="shared" si="4"/>
+        <v>37.9</v>
       </c>
       <c r="M24" s="1">
-        <f t="shared" ref="M24" si="5">AVERAGE(M4:M23)</f>
-        <v>1482.9459999999995</v>
+        <f t="shared" si="4"/>
+        <v>1858.9510000000005</v>
       </c>
       <c r="N24" s="1">
         <f>COUNTIF(N4:N23, "opt")</f>
-        <v>1</v>
-      </c>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="O24" s="1">
+        <f t="shared" ref="O24" si="5">AVERAGE(O4:O23)</f>
+        <v>38.9</v>
+      </c>
+      <c r="P24" s="1">
+        <f t="shared" ref="P24" si="6">AVERAGE(P4:P23)</f>
+        <v>1482.9459999999995</v>
+      </c>
+      <c r="Q24" s="1">
+        <f>COUNTIF(Q4:Q23, "opt")</f>
+        <v>1</v>
+      </c>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
         <v>31</v>
@@ -1620,8 +1856,11 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
         <v>27</v>
@@ -1630,22 +1869,27 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
@@ -1688,8 +1932,17 @@
       <c r="N28" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1709,34 +1962,44 @@
         <v>73</v>
       </c>
       <c r="G29">
-        <v>225.52</v>
+        <v>432.6</v>
       </c>
       <c r="H29" t="str">
         <f>IF($B29=F29, "opt", "")</f>
         <v/>
       </c>
       <c r="I29">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J29">
-        <v>2533.8000000000002</v>
+        <v>225.52</v>
       </c>
       <c r="K29" t="str">
         <f>IF($B29=I29, "opt", "")</f>
         <v/>
       </c>
       <c r="L29">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M29">
-        <v>2043.43</v>
+        <v>2533.8000000000002</v>
       </c>
       <c r="N29" t="str">
         <f>IF($B29=L29, "opt", "")</f>
         <v/>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <v>76</v>
+      </c>
+      <c r="P29">
+        <v>2043.43</v>
+      </c>
+      <c r="Q29" t="str">
+        <f>IF($B29=O29, "opt", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1753,37 +2016,47 @@
         <v>5.98</v>
       </c>
       <c r="F30">
+        <v>81</v>
+      </c>
+      <c r="G30">
+        <v>103.21</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" ref="H30:H48" si="7">IF($B30=F30, "opt", "")</f>
+        <v/>
+      </c>
+      <c r="I30">
         <v>77</v>
       </c>
-      <c r="G30">
+      <c r="J30">
         <v>2794.12</v>
       </c>
-      <c r="H30" t="str">
-        <f t="shared" ref="H30:H48" si="6">IF($B30=F30, "opt", "")</f>
-        <v/>
-      </c>
-      <c r="I30">
+      <c r="K30" t="str">
+        <f t="shared" ref="K30:K48" si="8">IF($B30=I30, "opt", "")</f>
+        <v/>
+      </c>
+      <c r="L30">
         <v>85</v>
       </c>
-      <c r="J30">
+      <c r="M30">
         <v>3605.84</v>
       </c>
-      <c r="K30" t="str">
-        <f t="shared" ref="K30:K48" si="7">IF($B30=I30, "opt", "")</f>
-        <v/>
-      </c>
-      <c r="L30">
+      <c r="N30" t="str">
+        <f t="shared" ref="N30:N48" si="9">IF($B30=L30, "opt", "")</f>
+        <v/>
+      </c>
+      <c r="O30">
         <v>90</v>
       </c>
-      <c r="M30">
+      <c r="P30">
         <v>1133.24</v>
       </c>
-      <c r="N30" t="str">
-        <f t="shared" ref="N30:N48" si="8">IF($B30=L30, "opt", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q30" t="str">
+        <f t="shared" ref="Q30:Q48" si="10">IF($B30=O30, "opt", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1803,34 +2076,44 @@
         <v>42</v>
       </c>
       <c r="G31">
+        <v>2097.8200000000002</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I31">
+        <v>42</v>
+      </c>
+      <c r="J31">
         <v>1185.19</v>
       </c>
-      <c r="H31" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I31">
+      <c r="K31" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L31">
         <v>44</v>
       </c>
-      <c r="J31">
+      <c r="M31">
         <v>3392.22</v>
       </c>
-      <c r="K31" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L31">
+      <c r="N31" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O31">
         <v>43</v>
       </c>
-      <c r="M31">
+      <c r="P31">
         <v>3591.99</v>
       </c>
-      <c r="N31" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q31" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -1847,37 +2130,47 @@
         <v>1.76</v>
       </c>
       <c r="F32">
+        <v>77</v>
+      </c>
+      <c r="G32">
+        <v>570.38</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I32">
         <v>75</v>
       </c>
-      <c r="G32">
+      <c r="J32">
         <v>766.05</v>
       </c>
-      <c r="H32" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I32">
+      <c r="K32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L32">
         <v>82</v>
       </c>
-      <c r="J32">
+      <c r="M32">
         <v>1957.88</v>
       </c>
-      <c r="K32" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L32">
+      <c r="N32" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O32">
         <v>81</v>
       </c>
-      <c r="M32">
+      <c r="P32">
         <v>2691.03</v>
       </c>
-      <c r="N32" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q32" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1897,34 +2190,44 @@
         <v>80</v>
       </c>
       <c r="G33">
+        <v>635.37</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I33">
+        <v>80</v>
+      </c>
+      <c r="J33">
         <v>1190.47</v>
       </c>
-      <c r="H33" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I33">
+      <c r="K33" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L33">
         <v>83</v>
       </c>
-      <c r="J33">
+      <c r="M33">
         <v>1721.95</v>
       </c>
-      <c r="K33" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L33">
+      <c r="N33" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O33">
         <v>86</v>
       </c>
-      <c r="M33">
+      <c r="P33">
         <v>2099.84</v>
       </c>
-      <c r="N33" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q33" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1944,34 +2247,44 @@
         <v>74</v>
       </c>
       <c r="G34">
+        <v>3556.53</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I34">
+        <v>74</v>
+      </c>
+      <c r="J34">
         <v>778.34</v>
       </c>
-      <c r="H34" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I34">
+      <c r="K34" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L34">
         <v>79</v>
       </c>
-      <c r="J34">
+      <c r="M34">
         <v>3138.24</v>
       </c>
-      <c r="K34" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L34">
+      <c r="N34" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O34">
         <v>77</v>
       </c>
-      <c r="M34">
+      <c r="P34">
         <v>2695.42</v>
       </c>
-      <c r="N34" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q34" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1988,37 +2301,47 @@
         <v>0.68</v>
       </c>
       <c r="F35">
+        <v>78</v>
+      </c>
+      <c r="G35">
+        <v>2232.29</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I35">
         <v>77</v>
       </c>
-      <c r="G35">
+      <c r="J35">
         <v>140.19</v>
       </c>
-      <c r="H35" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I35">
+      <c r="K35" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L35">
         <v>83</v>
       </c>
-      <c r="J35">
+      <c r="M35">
         <v>960.67</v>
       </c>
-      <c r="K35" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L35">
+      <c r="N35" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O35">
         <v>85</v>
       </c>
-      <c r="M35">
+      <c r="P35">
         <v>740.86</v>
       </c>
-      <c r="N35" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q35" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -2035,37 +2358,47 @@
         <v>1.29</v>
       </c>
       <c r="F36">
+        <v>94</v>
+      </c>
+      <c r="G36">
+        <v>1003.92</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I36">
         <v>95</v>
       </c>
-      <c r="G36">
+      <c r="J36">
         <v>2182.41</v>
       </c>
-      <c r="H36" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I36">
-        <v>98</v>
-      </c>
-      <c r="J36">
-        <v>873.59</v>
-      </c>
       <c r="K36" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="L36">
         <v>98</v>
       </c>
       <c r="M36">
+        <v>873.59</v>
+      </c>
+      <c r="N36" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O36">
+        <v>98</v>
+      </c>
+      <c r="P36">
         <v>3416.12</v>
       </c>
-      <c r="N36" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q36" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -2082,37 +2415,47 @@
         <v>1.01</v>
       </c>
       <c r="F37">
+        <v>82</v>
+      </c>
+      <c r="G37">
+        <v>2913.24</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I37">
         <v>81</v>
       </c>
-      <c r="G37">
+      <c r="J37">
         <v>1581.33</v>
       </c>
-      <c r="H37" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I37">
+      <c r="K37" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L37">
         <v>87</v>
       </c>
-      <c r="J37">
+      <c r="M37">
         <v>2964.31</v>
       </c>
-      <c r="K37" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L37">
+      <c r="N37" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O37">
         <v>88</v>
       </c>
-      <c r="M37">
+      <c r="P37">
         <v>2270.4899999999998</v>
       </c>
-      <c r="N37" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q37" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -2129,37 +2472,47 @@
         <v>7.58</v>
       </c>
       <c r="F38">
+        <v>78</v>
+      </c>
+      <c r="G38">
+        <v>1792.42</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I38">
         <v>76</v>
       </c>
-      <c r="G38">
+      <c r="J38">
         <v>1946.12</v>
       </c>
-      <c r="H38" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I38">
+      <c r="K38" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L38">
         <v>84</v>
       </c>
-      <c r="J38">
+      <c r="M38">
         <v>2067.7399999999998</v>
       </c>
-      <c r="K38" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L38">
+      <c r="N38" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O38">
         <v>85</v>
       </c>
-      <c r="M38">
+      <c r="P38">
         <v>2839.94</v>
       </c>
-      <c r="N38" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q38" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2176,37 +2529,47 @@
         <v>1.4</v>
       </c>
       <c r="F39">
+        <v>58</v>
+      </c>
+      <c r="G39">
+        <v>652.91999999999996</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I39">
         <v>60</v>
       </c>
-      <c r="G39">
+      <c r="J39">
         <v>178.08</v>
       </c>
-      <c r="H39" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I39">
+      <c r="K39" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L39">
         <v>64</v>
       </c>
-      <c r="J39">
+      <c r="M39">
         <v>2213.38</v>
       </c>
-      <c r="K39" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L39">
+      <c r="N39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O39">
         <v>63</v>
       </c>
-      <c r="M39">
+      <c r="P39">
         <v>1404.51</v>
       </c>
-      <c r="N39" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q39" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -2226,34 +2589,44 @@
         <v>79</v>
       </c>
       <c r="G40">
+        <v>2688.82</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I40">
+        <v>79</v>
+      </c>
+      <c r="J40">
         <v>1845.81</v>
       </c>
-      <c r="H40" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I40">
+      <c r="K40" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L40">
         <v>106</v>
       </c>
-      <c r="J40">
+      <c r="M40">
         <v>4030.49</v>
       </c>
-      <c r="K40" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L40">
+      <c r="N40" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O40">
         <v>88</v>
       </c>
-      <c r="M40">
+      <c r="P40">
         <v>2235.91</v>
       </c>
-      <c r="N40" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q40" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -2270,37 +2643,47 @@
         <v>1.25</v>
       </c>
       <c r="F41">
+        <v>86</v>
+      </c>
+      <c r="G41">
+        <v>2125.84</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I41">
         <v>85</v>
       </c>
-      <c r="G41">
+      <c r="J41">
         <v>2982.1</v>
       </c>
-      <c r="H41" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I41">
-        <v>88</v>
-      </c>
-      <c r="J41">
-        <v>758.9</v>
-      </c>
       <c r="K41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="L41">
         <v>88</v>
       </c>
       <c r="M41">
+        <v>758.9</v>
+      </c>
+      <c r="N41" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O41">
+        <v>88</v>
+      </c>
+      <c r="P41">
         <v>3032.11</v>
       </c>
-      <c r="N41" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q41" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -2317,37 +2700,47 @@
         <v>1.23</v>
       </c>
       <c r="F42">
+        <v>86</v>
+      </c>
+      <c r="G42">
+        <v>2935.53</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I42">
         <v>85</v>
       </c>
-      <c r="G42">
+      <c r="J42">
         <v>2435.9299999999998</v>
       </c>
-      <c r="H42" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I42">
+      <c r="K42" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L42">
         <v>92</v>
       </c>
-      <c r="J42">
+      <c r="M42">
         <v>2487.52</v>
       </c>
-      <c r="K42" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L42">
+      <c r="N42" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O42">
         <v>93</v>
       </c>
-      <c r="M42">
+      <c r="P42">
         <v>1500.97</v>
       </c>
-      <c r="N42" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q42" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -2367,34 +2760,44 @@
         <v>47</v>
       </c>
       <c r="G43">
-        <v>13.01</v>
+        <v>21.42</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>opt</v>
       </c>
       <c r="I43">
         <v>47</v>
       </c>
       <c r="J43">
+        <v>13.01</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="8"/>
+        <v>opt</v>
+      </c>
+      <c r="L43">
+        <v>47</v>
+      </c>
+      <c r="M43">
         <v>162.75</v>
       </c>
-      <c r="K43" t="str">
-        <f t="shared" si="7"/>
-        <v>opt</v>
-      </c>
-      <c r="L43">
+      <c r="N43" t="str">
+        <f t="shared" si="9"/>
+        <v>opt</v>
+      </c>
+      <c r="O43">
         <v>48</v>
       </c>
-      <c r="M43">
+      <c r="P43">
         <v>551.9</v>
       </c>
-      <c r="N43" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q43" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -2414,34 +2817,44 @@
         <v>63</v>
       </c>
       <c r="G44">
+        <v>348.49</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I44">
+        <v>63</v>
+      </c>
+      <c r="J44">
         <v>3516.79</v>
       </c>
-      <c r="H44" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I44">
+      <c r="K44" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L44">
         <v>66</v>
       </c>
-      <c r="J44">
+      <c r="M44">
         <v>3060.12</v>
       </c>
-      <c r="K44" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L44">
+      <c r="N44" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O44">
         <v>69</v>
       </c>
-      <c r="M44">
+      <c r="P44">
         <v>1302.26</v>
       </c>
-      <c r="N44" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q44" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -2461,34 +2874,44 @@
         <v>86</v>
       </c>
       <c r="G45">
+        <v>160.27000000000001</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I45">
+        <v>86</v>
+      </c>
+      <c r="J45">
         <v>2140.17</v>
       </c>
-      <c r="H45" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I45">
+      <c r="K45" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L45">
         <v>90</v>
       </c>
-      <c r="J45">
+      <c r="M45">
         <v>2247.27</v>
       </c>
-      <c r="K45" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L45">
+      <c r="N45" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O45">
         <v>91</v>
       </c>
-      <c r="M45">
+      <c r="P45">
         <v>2549.39</v>
       </c>
-      <c r="N45" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q45" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -2505,37 +2928,47 @@
         <v>0.45</v>
       </c>
       <c r="F46">
+        <v>51</v>
+      </c>
+      <c r="G46">
+        <v>2167.62</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I46">
         <v>50</v>
       </c>
-      <c r="G46">
+      <c r="J46">
         <v>3148.79</v>
       </c>
-      <c r="H46" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I46">
+      <c r="K46" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L46">
         <v>52</v>
       </c>
-      <c r="J46">
+      <c r="M46">
         <v>2009.49</v>
       </c>
-      <c r="K46" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L46">
+      <c r="N46" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O46">
         <v>53</v>
       </c>
-      <c r="M46">
+      <c r="P46">
         <v>162.55000000000001</v>
       </c>
-      <c r="N46" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q46" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -2555,34 +2988,44 @@
         <v>73</v>
       </c>
       <c r="G47">
+        <v>3294.1</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="7"/>
+        <v>opt</v>
+      </c>
+      <c r="I47">
+        <v>73</v>
+      </c>
+      <c r="J47">
         <v>248.24</v>
       </c>
-      <c r="H47" t="str">
-        <f t="shared" si="6"/>
-        <v>opt</v>
-      </c>
-      <c r="I47">
+      <c r="K47" t="str">
+        <f t="shared" si="8"/>
+        <v>opt</v>
+      </c>
+      <c r="L47">
         <v>75</v>
       </c>
-      <c r="J47">
+      <c r="M47">
         <v>3003.53</v>
       </c>
-      <c r="K47" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L47">
+      <c r="N47" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O47">
         <v>80</v>
       </c>
-      <c r="M47">
+      <c r="P47">
         <v>468.54</v>
       </c>
-      <c r="N47" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q47" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -2599,37 +3042,47 @@
         <v>1.35</v>
       </c>
       <c r="F48">
+        <v>69</v>
+      </c>
+      <c r="G48">
+        <v>21.14</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I48">
         <v>68</v>
       </c>
-      <c r="G48">
+      <c r="J48">
         <v>32.380000000000003</v>
       </c>
-      <c r="H48" t="str">
-        <f t="shared" si="6"/>
-        <v>opt</v>
-      </c>
-      <c r="I48">
+      <c r="K48" t="str">
+        <f t="shared" si="8"/>
+        <v>opt</v>
+      </c>
+      <c r="L48">
         <v>70</v>
       </c>
-      <c r="J48">
+      <c r="M48">
         <v>501.68</v>
       </c>
-      <c r="K48" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L48">
+      <c r="N48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O48">
         <v>68</v>
       </c>
-      <c r="M48">
+      <c r="P48">
         <v>1847.68</v>
       </c>
-      <c r="N48" t="str">
-        <f t="shared" si="8"/>
-        <v>opt</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q48" t="str">
+        <f t="shared" si="10"/>
+        <v>opt</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>30</v>
       </c>
@@ -2638,58 +3091,70 @@
         <v>70.45</v>
       </c>
       <c r="C49" s="1">
-        <f t="shared" ref="C49" si="9">AVERAGE(C29:C48)</f>
+        <f t="shared" ref="C49" si="11">AVERAGE(C29:C48)</f>
         <v>70.45</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" ref="D49" si="10">AVERAGE(D29:D48)</f>
+        <f t="shared" ref="D49" si="12">AVERAGE(D29:D48)</f>
         <v>1</v>
       </c>
       <c r="E49" s="1">
-        <f t="shared" ref="E49:G49" si="11">AVERAGE(E29:E48)</f>
+        <f t="shared" ref="E49:J49" si="13">AVERAGE(E29:E48)</f>
         <v>2.9030000000000005</v>
       </c>
       <c r="F49" s="1">
-        <f t="shared" si="11"/>
-        <v>72.3</v>
+        <f t="shared" si="13"/>
+        <v>72.849999999999994</v>
       </c>
       <c r="G49" s="1">
-        <f t="shared" si="11"/>
-        <v>1466.5520000000001</v>
+        <f t="shared" si="13"/>
+        <v>1487.6964999999998</v>
       </c>
       <c r="H49" s="1">
         <f>COUNTIF(H29:H48, "opt")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" ref="I49" si="12">AVERAGE(I29:I48)</f>
-        <v>77.599999999999994</v>
+        <f t="shared" si="13"/>
+        <v>72.3</v>
       </c>
       <c r="J49" s="1">
-        <f t="shared" ref="J49" si="13">AVERAGE(J29:J48)</f>
-        <v>2184.5685000000003</v>
+        <f t="shared" si="13"/>
+        <v>1466.5520000000001</v>
       </c>
       <c r="K49" s="1">
         <f>COUNTIF(K29:K48, "opt")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L49" s="1">
         <f t="shared" ref="L49" si="14">AVERAGE(L29:L48)</f>
-        <v>77.5</v>
+        <v>77.599999999999994</v>
       </c>
       <c r="M49" s="1">
         <f t="shared" ref="M49" si="15">AVERAGE(M29:M48)</f>
-        <v>1928.9090000000001</v>
+        <v>2184.5685000000003</v>
       </c>
       <c r="N49" s="1">
         <f>COUNTIF(N29:N48, "opt")</f>
         <v>1</v>
       </c>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O49" s="1">
+        <f t="shared" ref="O49" si="16">AVERAGE(O29:O48)</f>
+        <v>77.5</v>
+      </c>
+      <c r="P49" s="1">
+        <f t="shared" ref="P49" si="17">AVERAGE(P29:P48)</f>
+        <v>1928.9090000000001</v>
+      </c>
+      <c r="Q49" s="1">
+        <f>COUNTIF(Q29:Q48, "opt")</f>
+        <v>1</v>
+      </c>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2" t="s">
         <v>33</v>
@@ -2706,8 +3171,11 @@
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2" t="s">
         <v>27</v>
@@ -2716,22 +3184,27 @@
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O52" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>20</v>
       </c>
@@ -2774,8 +3247,17 @@
       <c r="N53" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q53" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -2792,37 +3274,47 @@
         <v>3608.26</v>
       </c>
       <c r="F54">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G54">
-        <v>657.06</v>
+        <v>254.58</v>
       </c>
       <c r="H54" t="str">
         <f>IF($B54=F54, "opt", "")</f>
         <v/>
       </c>
       <c r="I54">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="J54">
-        <v>631.5</v>
+        <v>657.06</v>
       </c>
       <c r="K54" t="str">
         <f>IF($B54=I54, "opt", "")</f>
         <v/>
       </c>
       <c r="L54">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M54">
-        <v>2862.68</v>
+        <v>631.5</v>
       </c>
       <c r="N54" t="str">
         <f>IF($B54=L54, "opt", "")</f>
         <v/>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O54">
+        <v>149</v>
+      </c>
+      <c r="P54">
+        <v>2862.68</v>
+      </c>
+      <c r="Q54" t="str">
+        <f>IF($B54=O54, "opt", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1</v>
       </c>
@@ -2839,37 +3331,47 @@
         <v>1985.8</v>
       </c>
       <c r="F55">
+        <v>154</v>
+      </c>
+      <c r="G55">
+        <v>2386.46</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" ref="H55:H74" si="18">IF($B55=F55, "opt", "")</f>
+        <v/>
+      </c>
+      <c r="I55">
         <v>152</v>
       </c>
-      <c r="G55">
+      <c r="J55">
         <v>2672.73</v>
       </c>
-      <c r="H55" t="str">
-        <f t="shared" ref="H55:H73" si="16">IF($B55=F55, "opt", "")</f>
-        <v/>
-      </c>
-      <c r="I55">
+      <c r="K55" t="str">
+        <f t="shared" ref="K55:K73" si="19">IF($B55=I55, "opt", "")</f>
+        <v/>
+      </c>
+      <c r="L55">
         <v>182</v>
       </c>
-      <c r="J55">
+      <c r="M55">
         <v>3637.73</v>
       </c>
-      <c r="K55" t="str">
-        <f t="shared" ref="K55:K73" si="17">IF($B55=I55, "opt", "")</f>
-        <v/>
-      </c>
-      <c r="L55">
+      <c r="N55" t="str">
+        <f t="shared" ref="N55:N73" si="20">IF($B55=L55, "opt", "")</f>
+        <v/>
+      </c>
+      <c r="O55">
         <v>169</v>
       </c>
-      <c r="M55">
+      <c r="P55">
         <v>2837.51</v>
       </c>
-      <c r="N55" t="str">
-        <f t="shared" ref="N55:N73" si="18">IF($B55=L55, "opt", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q55" t="str">
+        <f t="shared" ref="Q55:Q73" si="21">IF($B55=O55, "opt", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -2886,37 +3388,47 @@
         <v>179.16</v>
       </c>
       <c r="F56">
+        <v>83</v>
+      </c>
+      <c r="G56">
+        <v>309.95999999999998</v>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I56">
         <v>82</v>
       </c>
-      <c r="G56">
+      <c r="J56">
         <v>1015.5</v>
       </c>
-      <c r="H56" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I56">
+      <c r="K56" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="L56">
         <v>89</v>
       </c>
-      <c r="J56">
+      <c r="M56">
         <v>714.64</v>
       </c>
-      <c r="K56" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="L56">
+      <c r="N56" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O56">
         <v>87</v>
       </c>
-      <c r="M56">
+      <c r="P56">
         <v>3470.98</v>
       </c>
-      <c r="N56" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q56" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>3</v>
       </c>
@@ -2933,37 +3445,47 @@
         <v>3631.76</v>
       </c>
       <c r="F57">
+        <v>154</v>
+      </c>
+      <c r="G57">
+        <v>2378.6999999999998</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I57">
         <v>151</v>
       </c>
-      <c r="G57">
+      <c r="J57">
         <v>1923.96</v>
       </c>
-      <c r="H57" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I57">
+      <c r="K57" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="L57">
         <v>165</v>
       </c>
-      <c r="J57">
+      <c r="M57">
         <v>3447.42</v>
       </c>
-      <c r="K57" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="L57">
+      <c r="N57" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O57">
         <v>162</v>
       </c>
-      <c r="M57">
+      <c r="P57">
         <v>1616.56</v>
       </c>
-      <c r="N57" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q57" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -2980,37 +3502,47 @@
         <v>911.98</v>
       </c>
       <c r="F58">
+        <v>165</v>
+      </c>
+      <c r="G58">
+        <v>648.26</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I58">
         <v>160</v>
       </c>
-      <c r="G58">
+      <c r="J58">
         <v>2621.15</v>
       </c>
-      <c r="H58" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I58">
+      <c r="K58" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="L58">
         <v>168</v>
       </c>
-      <c r="J58">
+      <c r="M58">
         <v>1174.47</v>
       </c>
-      <c r="K58" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="L58">
+      <c r="N58" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O58">
         <v>165</v>
       </c>
-      <c r="M58">
+      <c r="P58">
         <v>2670.1</v>
       </c>
-      <c r="N58" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q58" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -3027,37 +3559,47 @@
         <v>3604.64</v>
       </c>
       <c r="F59">
+        <v>154</v>
+      </c>
+      <c r="G59">
+        <v>1211.22</v>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I59">
         <v>152</v>
       </c>
-      <c r="G59">
+      <c r="J59">
         <v>1347.62</v>
       </c>
-      <c r="H59" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I59">
+      <c r="K59" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="L59">
         <v>162</v>
       </c>
-      <c r="J59">
+      <c r="M59">
         <v>1435.66</v>
       </c>
-      <c r="K59" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="L59">
+      <c r="N59" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O59">
         <v>159</v>
       </c>
-      <c r="M59">
+      <c r="P59">
         <v>3351.26</v>
       </c>
-      <c r="N59" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q59" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -3074,37 +3616,47 @@
         <v>3655.54</v>
       </c>
       <c r="F60">
+        <v>162</v>
+      </c>
+      <c r="G60">
+        <v>1868.42</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I60">
         <v>160</v>
       </c>
-      <c r="G60">
+      <c r="J60">
         <v>1825.03</v>
       </c>
-      <c r="H60" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I60">
+      <c r="K60" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="L60">
         <v>169</v>
       </c>
-      <c r="J60">
+      <c r="M60">
         <v>1391.51</v>
       </c>
-      <c r="K60" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="L60">
+      <c r="N60" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O60">
         <v>172</v>
       </c>
-      <c r="M60">
+      <c r="P60">
         <v>2752.16</v>
       </c>
-      <c r="N60" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q60" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -3121,37 +3673,47 @@
         <v>3648.06</v>
       </c>
       <c r="F61">
+        <v>177</v>
+      </c>
+      <c r="G61">
+        <v>3139.32</v>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I61">
         <v>180</v>
       </c>
-      <c r="G61">
+      <c r="J61">
         <v>2940.9</v>
       </c>
-      <c r="H61" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I61">
+      <c r="K61" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="L61">
         <v>190</v>
       </c>
-      <c r="J61">
+      <c r="M61">
         <v>1329.91</v>
       </c>
-      <c r="K61" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="L61">
+      <c r="N61" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O61">
         <v>185</v>
       </c>
-      <c r="M61">
+      <c r="P61">
         <v>1546.74</v>
       </c>
-      <c r="N61" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q61" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -3171,34 +3733,44 @@
         <v>156</v>
       </c>
       <c r="G62">
+        <v>1556.14</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I62">
+        <v>156</v>
+      </c>
+      <c r="J62">
         <v>1724.02</v>
       </c>
-      <c r="H62" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I62">
-        <v>166</v>
-      </c>
-      <c r="J62">
-        <v>3240.09</v>
-      </c>
       <c r="K62" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="L62">
         <v>166</v>
       </c>
       <c r="M62">
+        <v>3240.09</v>
+      </c>
+      <c r="N62" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O62">
+        <v>166</v>
+      </c>
+      <c r="P62">
         <v>3490.77</v>
       </c>
-      <c r="N62" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q62" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>9</v>
       </c>
@@ -3215,37 +3787,47 @@
         <v>3602.38</v>
       </c>
       <c r="F63">
+        <v>153</v>
+      </c>
+      <c r="G63">
+        <v>3116.66</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I63">
         <v>155</v>
       </c>
-      <c r="G63">
+      <c r="J63">
         <v>1856.66</v>
       </c>
-      <c r="H63" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I63">
+      <c r="K63" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="L63">
         <v>162</v>
       </c>
-      <c r="J63">
+      <c r="M63">
         <v>3571.87</v>
       </c>
-      <c r="K63" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="L63">
+      <c r="N63" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O63">
         <v>165</v>
       </c>
-      <c r="M63">
+      <c r="P63">
         <v>2597.0500000000002</v>
       </c>
-      <c r="N63" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q63" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -3262,37 +3844,47 @@
         <v>338.36</v>
       </c>
       <c r="F64">
+        <v>117</v>
+      </c>
+      <c r="G64">
+        <v>1565.52</v>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I64">
         <v>114</v>
       </c>
-      <c r="G64">
+      <c r="J64">
         <v>2136.59</v>
       </c>
-      <c r="H64" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I64">
+      <c r="K64" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="L64">
         <v>125</v>
       </c>
-      <c r="J64">
+      <c r="M64">
         <v>2636.94</v>
       </c>
-      <c r="K64" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="L64">
+      <c r="N64" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O64">
         <v>124</v>
       </c>
-      <c r="M64">
+      <c r="P64">
         <v>3155.58</v>
       </c>
-      <c r="N64" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q64" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>11</v>
       </c>
@@ -3309,37 +3901,47 @@
         <v>3620.36</v>
       </c>
       <c r="F65">
+        <v>162</v>
+      </c>
+      <c r="G65">
+        <v>882.17</v>
+      </c>
+      <c r="H65" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I65">
         <v>160</v>
       </c>
-      <c r="G65">
+      <c r="J65">
         <v>956.97</v>
       </c>
-      <c r="H65" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I65">
+      <c r="K65" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="L65">
         <v>214</v>
       </c>
-      <c r="J65">
+      <c r="M65">
         <v>5236.25</v>
       </c>
-      <c r="K65" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="L65">
+      <c r="N65" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O65">
         <v>173</v>
       </c>
-      <c r="M65">
+      <c r="P65">
         <v>3430.55</v>
       </c>
-      <c r="N65" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q65" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -3356,37 +3958,47 @@
         <v>913.1</v>
       </c>
       <c r="F66">
+        <v>156</v>
+      </c>
+      <c r="G66">
+        <v>3508.34</v>
+      </c>
+      <c r="H66" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I66">
         <v>158</v>
       </c>
-      <c r="G66">
+      <c r="J66">
         <v>2765.03</v>
       </c>
-      <c r="H66" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I66">
+      <c r="K66" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="L66">
         <v>166</v>
       </c>
-      <c r="J66">
+      <c r="M66">
         <v>1399.34</v>
       </c>
-      <c r="K66" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="L66">
+      <c r="N66" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O66">
         <v>164</v>
       </c>
-      <c r="M66">
+      <c r="P66">
         <v>2690.94</v>
       </c>
-      <c r="N66" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q66" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>13</v>
       </c>
@@ -3403,37 +4015,47 @@
         <v>236.64</v>
       </c>
       <c r="F67">
+        <v>172</v>
+      </c>
+      <c r="G67">
+        <v>1535.47</v>
+      </c>
+      <c r="H67" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I67">
         <v>168</v>
       </c>
-      <c r="G67">
+      <c r="J67">
         <v>3493.09</v>
       </c>
-      <c r="H67" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I67">
+      <c r="K67" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="L67">
         <v>191</v>
       </c>
-      <c r="J67">
+      <c r="M67">
         <v>3558.47</v>
       </c>
-      <c r="K67" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="L67">
+      <c r="N67" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O67">
         <v>184</v>
       </c>
-      <c r="M67">
+      <c r="P67">
         <v>1410.68</v>
       </c>
-      <c r="N67" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q67" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -3450,37 +4072,47 @@
         <v>17.079999999999998</v>
       </c>
       <c r="F68">
+        <v>89</v>
+      </c>
+      <c r="G68">
+        <v>1872.38</v>
+      </c>
+      <c r="H68" t="str">
+        <f t="shared" si="18"/>
+        <v>opt</v>
+      </c>
+      <c r="I68">
         <v>90</v>
       </c>
-      <c r="G68">
+      <c r="J68">
         <v>20.65</v>
       </c>
-      <c r="H68" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I68">
+      <c r="K68" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="L68">
         <v>93</v>
       </c>
-      <c r="J68">
+      <c r="M68">
         <v>2570.6</v>
       </c>
-      <c r="K68" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="L68">
+      <c r="N68" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O68">
         <v>91</v>
       </c>
-      <c r="M68">
+      <c r="P68">
         <v>894.18</v>
       </c>
-      <c r="N68" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q68" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -3500,34 +4132,44 @@
         <v>121</v>
       </c>
       <c r="G69">
+        <v>1535.21</v>
+      </c>
+      <c r="H69" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I69">
+        <v>121</v>
+      </c>
+      <c r="J69">
         <v>3062.52</v>
       </c>
-      <c r="H69" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I69">
+      <c r="K69" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="L69">
         <v>128</v>
       </c>
-      <c r="J69">
+      <c r="M69">
         <v>2018.32</v>
       </c>
-      <c r="K69" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="L69">
+      <c r="N69" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O69">
         <v>127</v>
       </c>
-      <c r="M69">
+      <c r="P69">
         <v>3492.04</v>
       </c>
-      <c r="N69" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q69" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -3547,34 +4189,44 @@
         <v>166</v>
       </c>
       <c r="G70">
+        <v>3144.44</v>
+      </c>
+      <c r="H70" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I70">
+        <v>166</v>
+      </c>
+      <c r="J70">
         <v>1031.4100000000001</v>
       </c>
-      <c r="H70" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I70">
-        <v>180</v>
-      </c>
-      <c r="J70">
-        <v>2915.07</v>
-      </c>
       <c r="K70" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="L70">
         <v>180</v>
       </c>
       <c r="M70">
+        <v>2915.07</v>
+      </c>
+      <c r="N70" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O70">
+        <v>180</v>
+      </c>
+      <c r="P70">
         <v>2578.83</v>
       </c>
-      <c r="N70" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q70" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>17</v>
       </c>
@@ -3591,37 +4243,47 @@
         <v>53.23</v>
       </c>
       <c r="F71">
+        <v>99</v>
+      </c>
+      <c r="G71">
+        <v>1565.23</v>
+      </c>
+      <c r="H71" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I71">
         <v>101</v>
       </c>
-      <c r="G71">
+      <c r="J71">
         <v>351.49</v>
       </c>
-      <c r="H71" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I71">
+      <c r="K71" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="L71">
         <v>104</v>
       </c>
-      <c r="J71">
+      <c r="M71">
         <v>891.9</v>
       </c>
-      <c r="K71" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="L71">
+      <c r="N71" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O71">
         <v>100</v>
       </c>
-      <c r="M71">
+      <c r="P71">
         <v>1374.47</v>
       </c>
-      <c r="N71" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q71" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>18</v>
       </c>
@@ -3641,34 +4303,44 @@
         <v>144</v>
       </c>
       <c r="G72">
+        <v>927.05</v>
+      </c>
+      <c r="H72" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I72">
+        <v>144</v>
+      </c>
+      <c r="J72">
         <v>903.06</v>
       </c>
-      <c r="H72" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I72">
-        <v>151</v>
-      </c>
-      <c r="J72">
-        <v>1895.86</v>
-      </c>
       <c r="K72" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="L72">
         <v>151</v>
       </c>
       <c r="M72">
+        <v>1895.86</v>
+      </c>
+      <c r="N72" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O72">
+        <v>151</v>
+      </c>
+      <c r="P72">
         <v>3455.11</v>
       </c>
-      <c r="N72" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q72" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>19</v>
       </c>
@@ -3685,37 +4357,47 @@
         <v>31.71</v>
       </c>
       <c r="F73">
+        <v>132</v>
+      </c>
+      <c r="G73">
+        <v>2536.19</v>
+      </c>
+      <c r="H73" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="I73">
         <v>131</v>
       </c>
-      <c r="G73">
+      <c r="J73">
         <v>2013.01</v>
       </c>
-      <c r="H73" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I73">
+      <c r="K73" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="L73">
         <v>142</v>
       </c>
-      <c r="J73">
+      <c r="M73">
         <v>1693.27</v>
       </c>
-      <c r="K73" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="L73">
+      <c r="N73" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="O73">
         <v>139</v>
       </c>
-      <c r="M73">
+      <c r="P73">
         <v>1350.2</v>
       </c>
-      <c r="N73" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q73" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>30</v>
       </c>
@@ -3724,74 +4406,89 @@
         <v>136.05000000000001</v>
       </c>
       <c r="C74" s="1">
-        <f t="shared" ref="C74" si="19">AVERAGE(C54:C73)</f>
+        <f t="shared" ref="C74" si="22">AVERAGE(C54:C73)</f>
         <v>135.35</v>
       </c>
       <c r="D74" s="1">
-        <f t="shared" ref="D74" si="20">AVERAGE(D54:D73)</f>
+        <f t="shared" ref="D74" si="23">AVERAGE(D54:D73)</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="E74" s="1">
-        <f t="shared" ref="E74:G74" si="21">AVERAGE(E54:E73)</f>
+        <f t="shared" ref="E74:J74" si="24">AVERAGE(E54:E73)</f>
         <v>1894.1545000000006</v>
       </c>
       <c r="F74" s="1">
-        <f t="shared" si="21"/>
-        <v>142.15</v>
+        <f t="shared" si="24"/>
+        <v>143</v>
       </c>
       <c r="G74" s="1">
-        <f t="shared" si="21"/>
-        <v>1765.9225000000001</v>
+        <f t="shared" si="24"/>
+        <v>1797.086</v>
       </c>
       <c r="H74" s="1">
         <f>COUNTIF(H54:H73, "opt")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I74" s="1">
-        <f t="shared" ref="I74" si="22">AVERAGE(I54:I73)</f>
-        <v>154.85</v>
+        <f t="shared" si="24"/>
+        <v>142.15</v>
       </c>
       <c r="J74" s="1">
-        <f t="shared" ref="J74" si="23">AVERAGE(J54:J73)</f>
-        <v>2269.5409999999997</v>
+        <f t="shared" si="24"/>
+        <v>1765.9225000000001</v>
       </c>
       <c r="K74" s="1">
         <f>COUNTIF(K54:K73, "opt")</f>
         <v>0</v>
       </c>
       <c r="L74" s="1">
-        <f t="shared" ref="L74" si="24">AVERAGE(L54:L73)</f>
-        <v>150.6</v>
+        <f t="shared" ref="L74" si="25">AVERAGE(L54:L73)</f>
+        <v>154.85</v>
       </c>
       <c r="M74" s="1">
-        <f t="shared" ref="M74" si="25">AVERAGE(M54:M73)</f>
-        <v>2551.4195000000004</v>
+        <f t="shared" ref="M74" si="26">AVERAGE(M54:M73)</f>
+        <v>2269.5409999999997</v>
       </c>
       <c r="N74" s="1">
         <f>COUNTIF(N54:N73, "opt")</f>
         <v>0</v>
       </c>
+      <c r="O74" s="1">
+        <f t="shared" ref="O74" si="27">AVERAGE(O54:O73)</f>
+        <v>150.6</v>
+      </c>
+      <c r="P74" s="1">
+        <f t="shared" ref="P74" si="28">AVERAGE(P54:P73)</f>
+        <v>2551.4195000000004</v>
+      </c>
+      <c r="Q74" s="1">
+        <f>COUNTIF(Q54:Q73, "opt")</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Q1:S74">
-    <sortCondition ref="Q1:Q74"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="T1:V20">
+    <sortCondition ref="T1:T20"/>
   </sortState>
-  <mergeCells count="15">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="B1:N1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B51:N51"/>
+  <mergeCells count="18">
+    <mergeCell ref="B51:Q51"/>
     <mergeCell ref="B52:E52"/>
+    <mergeCell ref="L52:N52"/>
+    <mergeCell ref="O52:Q52"/>
+    <mergeCell ref="B26:Q26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="O27:Q27"/>
+    <mergeCell ref="I27:K27"/>
     <mergeCell ref="I52:K52"/>
-    <mergeCell ref="L52:N52"/>
-    <mergeCell ref="B26:N26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="L27:N27"/>
     <mergeCell ref="F27:H27"/>
     <mergeCell ref="F52:H52"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Testing with new fitness finished.
</commit_message>
<xml_diff>
--- a/algorithms/results/comparison.xlsx
+++ b/algorithms/results/comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\akcijanje\nauka\moji radovi\aktivno\k-domination\algorithms\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744D1327-B6CD-4D3E-95D6-CBB0B9D8A4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8329C47-A419-462B-8E95-B5B6934F41DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3555" windowWidth="29040" windowHeight="15840" xr2:uid="{9811A06C-B274-406A-BE4D-18F0FA4A89B1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="38">
   <si>
     <t>bath.txt</t>
   </si>
@@ -520,7 +520,7 @@
   <dimension ref="A1:Z74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="Y1" sqref="Y1:AA1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2343,9 +2343,11 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="F27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
       <c r="I27" s="3" t="s">
         <v>36</v>
       </c>
@@ -2388,9 +2390,15 @@
       <c r="E28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="I28" s="1" t="s">
         <v>22</v>
       </c>
@@ -2453,6 +2461,16 @@
       <c r="E29">
         <v>0.69</v>
       </c>
+      <c r="F29">
+        <v>71</v>
+      </c>
+      <c r="G29">
+        <v>428.91</v>
+      </c>
+      <c r="H29" t="str">
+        <f>IF($B29=F29, "opt", "")</f>
+        <v>opt</v>
+      </c>
       <c r="I29">
         <v>72</v>
       </c>
@@ -2505,7 +2523,7 @@
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B30">
@@ -2520,6 +2538,16 @@
       <c r="E30">
         <v>5.98</v>
       </c>
+      <c r="F30">
+        <v>76</v>
+      </c>
+      <c r="G30">
+        <v>1378.74</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" ref="H30:H48" si="9">IF($B30=F30, "opt", "")</f>
+        <v>opt</v>
+      </c>
       <c r="I30">
         <v>79</v>
       </c>
@@ -2527,7 +2555,7 @@
         <v>2548.89</v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" ref="K30:K48" si="9">IF($B30=I30, "opt", "")</f>
+        <f t="shared" ref="K30:K48" si="10">IF($B30=I30, "opt", "")</f>
         <v/>
       </c>
       <c r="L30">
@@ -2537,7 +2565,7 @@
         <v>103.21</v>
       </c>
       <c r="N30" t="str">
-        <f t="shared" ref="N30:N48" si="10">IF($B30=L30, "opt", "")</f>
+        <f t="shared" ref="N30:N48" si="11">IF($B30=L30, "opt", "")</f>
         <v/>
       </c>
       <c r="O30">
@@ -2547,7 +2575,7 @@
         <v>2794.12</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" ref="Q30:Q48" si="11">IF($B30=O30, "opt", "")</f>
+        <f t="shared" ref="Q30:Q48" si="12">IF($B30=O30, "opt", "")</f>
         <v/>
       </c>
       <c r="R30">
@@ -2557,7 +2585,7 @@
         <v>3605.84</v>
       </c>
       <c r="T30" t="str">
-        <f t="shared" ref="T30:T48" si="12">IF($B30=R30, "opt", "")</f>
+        <f t="shared" ref="T30:T48" si="13">IF($B30=R30, "opt", "")</f>
         <v/>
       </c>
       <c r="U30">
@@ -2567,7 +2595,7 @@
         <v>1133.24</v>
       </c>
       <c r="W30" t="str">
-        <f t="shared" ref="W30:W48" si="13">IF($B30=U30, "opt", "")</f>
+        <f t="shared" ref="W30:W48" si="14">IF($B30=U30, "opt", "")</f>
         <v/>
       </c>
     </row>
@@ -2587,6 +2615,16 @@
       <c r="E31">
         <v>0.91</v>
       </c>
+      <c r="F31">
+        <v>40</v>
+      </c>
+      <c r="G31">
+        <v>427.46</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="9"/>
+        <v>opt</v>
+      </c>
       <c r="I31">
         <v>41</v>
       </c>
@@ -2594,7 +2632,7 @@
         <v>1719.25</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L31">
@@ -2604,7 +2642,7 @@
         <v>2097.8200000000002</v>
       </c>
       <c r="N31" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O31">
@@ -2614,7 +2652,7 @@
         <v>1185.19</v>
       </c>
       <c r="Q31" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="R31">
@@ -2624,7 +2662,7 @@
         <v>3392.22</v>
       </c>
       <c r="T31" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U31">
@@ -2634,7 +2672,7 @@
         <v>3591.99</v>
       </c>
       <c r="W31" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -2654,6 +2692,16 @@
       <c r="E32">
         <v>1.76</v>
       </c>
+      <c r="F32">
+        <v>74</v>
+      </c>
+      <c r="G32">
+        <v>589.64</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
       <c r="I32">
         <v>74</v>
       </c>
@@ -2661,7 +2709,7 @@
         <v>181.98</v>
       </c>
       <c r="K32" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L32">
@@ -2671,7 +2719,7 @@
         <v>570.38</v>
       </c>
       <c r="N32" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O32">
@@ -2681,7 +2729,7 @@
         <v>766.05</v>
       </c>
       <c r="Q32" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="R32">
@@ -2691,7 +2739,7 @@
         <v>1957.88</v>
       </c>
       <c r="T32" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U32">
@@ -2701,12 +2749,12 @@
         <v>2691.03</v>
       </c>
       <c r="W32" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B33">
@@ -2721,6 +2769,16 @@
       <c r="E33">
         <v>0.95</v>
       </c>
+      <c r="F33">
+        <v>78</v>
+      </c>
+      <c r="G33">
+        <v>2040.22</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="9"/>
+        <v>opt</v>
+      </c>
       <c r="I33">
         <v>80</v>
       </c>
@@ -2728,7 +2786,7 @@
         <v>36.42</v>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L33">
@@ -2738,7 +2796,7 @@
         <v>635.37</v>
       </c>
       <c r="N33" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O33">
@@ -2748,7 +2806,7 @@
         <v>1190.47</v>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="R33">
@@ -2758,7 +2816,7 @@
         <v>1721.95</v>
       </c>
       <c r="T33" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U33">
@@ -2768,7 +2826,7 @@
         <v>2099.84</v>
       </c>
       <c r="W33" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -2788,6 +2846,16 @@
       <c r="E34">
         <v>1.53</v>
       </c>
+      <c r="F34">
+        <v>73</v>
+      </c>
+      <c r="G34">
+        <v>1008.36</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
       <c r="I34">
         <v>73</v>
       </c>
@@ -2795,7 +2863,7 @@
         <v>568.61</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L34">
@@ -2805,7 +2873,7 @@
         <v>3556.53</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O34">
@@ -2815,7 +2883,7 @@
         <v>778.34</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="R34">
@@ -2825,7 +2893,7 @@
         <v>3138.24</v>
       </c>
       <c r="T34" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U34">
@@ -2835,12 +2903,12 @@
         <v>2695.42</v>
       </c>
       <c r="W34" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B35">
@@ -2855,6 +2923,16 @@
       <c r="E35">
         <v>0.68</v>
       </c>
+      <c r="F35">
+        <v>76</v>
+      </c>
+      <c r="G35">
+        <v>3453.05</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="9"/>
+        <v>opt</v>
+      </c>
       <c r="I35">
         <v>79</v>
       </c>
@@ -2862,7 +2940,7 @@
         <v>110.55</v>
       </c>
       <c r="K35" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L35">
@@ -2872,7 +2950,7 @@
         <v>2232.29</v>
       </c>
       <c r="N35" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O35">
@@ -2882,7 +2960,7 @@
         <v>140.19</v>
       </c>
       <c r="Q35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="R35">
@@ -2892,7 +2970,7 @@
         <v>960.67</v>
       </c>
       <c r="T35" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U35">
@@ -2902,7 +2980,7 @@
         <v>740.86</v>
       </c>
       <c r="W35" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -2922,6 +3000,16 @@
       <c r="E36">
         <v>1.29</v>
       </c>
+      <c r="F36">
+        <v>94</v>
+      </c>
+      <c r="G36">
+        <v>600.54999999999995</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
       <c r="I36">
         <v>93</v>
       </c>
@@ -2929,7 +3017,7 @@
         <v>991.51</v>
       </c>
       <c r="K36" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>opt</v>
       </c>
       <c r="L36">
@@ -2939,7 +3027,7 @@
         <v>1003.92</v>
       </c>
       <c r="N36" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O36">
@@ -2949,7 +3037,7 @@
         <v>2182.41</v>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="R36">
@@ -2959,7 +3047,7 @@
         <v>873.59</v>
       </c>
       <c r="T36" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U36">
@@ -2969,7 +3057,7 @@
         <v>3416.12</v>
       </c>
       <c r="W36" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -2989,6 +3077,16 @@
       <c r="E37">
         <v>1.01</v>
       </c>
+      <c r="F37">
+        <v>79</v>
+      </c>
+      <c r="G37">
+        <v>2058.4499999999998</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
       <c r="I37">
         <v>81</v>
       </c>
@@ -2996,7 +3094,7 @@
         <v>694.69</v>
       </c>
       <c r="K37" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L37">
@@ -3006,7 +3104,7 @@
         <v>2913.24</v>
       </c>
       <c r="N37" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O37">
@@ -3016,7 +3114,7 @@
         <v>1581.33</v>
       </c>
       <c r="Q37" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="R37">
@@ -3026,7 +3124,7 @@
         <v>2964.31</v>
       </c>
       <c r="T37" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U37">
@@ -3036,12 +3134,12 @@
         <v>2270.4899999999998</v>
       </c>
       <c r="W37" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B38">
@@ -3056,6 +3154,16 @@
       <c r="E38">
         <v>7.58</v>
       </c>
+      <c r="F38">
+        <v>75</v>
+      </c>
+      <c r="G38">
+        <v>1014.11</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="9"/>
+        <v>opt</v>
+      </c>
       <c r="I38">
         <v>76</v>
       </c>
@@ -3063,7 +3171,7 @@
         <v>893.4</v>
       </c>
       <c r="K38" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L38">
@@ -3073,7 +3181,7 @@
         <v>1792.42</v>
       </c>
       <c r="N38" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O38">
@@ -3083,7 +3191,7 @@
         <v>1946.12</v>
       </c>
       <c r="Q38" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="R38">
@@ -3093,7 +3201,7 @@
         <v>2067.7399999999998</v>
       </c>
       <c r="T38" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U38">
@@ -3103,7 +3211,7 @@
         <v>2839.94</v>
       </c>
       <c r="W38" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -3123,6 +3231,16 @@
       <c r="E39">
         <v>1.4</v>
       </c>
+      <c r="F39">
+        <v>57</v>
+      </c>
+      <c r="G39">
+        <v>212.52</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
       <c r="I39">
         <v>57</v>
       </c>
@@ -3130,7 +3248,7 @@
         <v>1920.49</v>
       </c>
       <c r="K39" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L39">
@@ -3140,7 +3258,7 @@
         <v>652.91999999999996</v>
       </c>
       <c r="N39" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O39">
@@ -3150,7 +3268,7 @@
         <v>178.08</v>
       </c>
       <c r="Q39" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="R39">
@@ -3160,7 +3278,7 @@
         <v>2213.38</v>
       </c>
       <c r="T39" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U39">
@@ -3170,7 +3288,7 @@
         <v>1404.51</v>
       </c>
       <c r="W39" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -3190,6 +3308,16 @@
       <c r="E40">
         <v>24.5</v>
       </c>
+      <c r="F40">
+        <v>78</v>
+      </c>
+      <c r="G40">
+        <v>467.45</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
       <c r="I40">
         <v>78</v>
       </c>
@@ -3197,7 +3325,7 @@
         <v>3577.82</v>
       </c>
       <c r="K40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L40">
@@ -3207,7 +3335,7 @@
         <v>2688.82</v>
       </c>
       <c r="N40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O40">
@@ -3217,7 +3345,7 @@
         <v>1845.81</v>
       </c>
       <c r="Q40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="R40">
@@ -3227,7 +3355,7 @@
         <v>4030.49</v>
       </c>
       <c r="T40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U40">
@@ -3237,12 +3365,12 @@
         <v>2235.91</v>
       </c>
       <c r="W40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B41">
@@ -3257,6 +3385,16 @@
       <c r="E41">
         <v>1.25</v>
       </c>
+      <c r="F41">
+        <v>83</v>
+      </c>
+      <c r="G41">
+        <v>1723.67</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="9"/>
+        <v>opt</v>
+      </c>
       <c r="I41">
         <v>84</v>
       </c>
@@ -3264,7 +3402,7 @@
         <v>1653.61</v>
       </c>
       <c r="K41" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L41">
@@ -3274,7 +3412,7 @@
         <v>2125.84</v>
       </c>
       <c r="N41" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O41">
@@ -3284,7 +3422,7 @@
         <v>2982.1</v>
       </c>
       <c r="Q41" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="R41">
@@ -3294,7 +3432,7 @@
         <v>758.9</v>
       </c>
       <c r="T41" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U41">
@@ -3304,7 +3442,7 @@
         <v>3032.11</v>
       </c>
       <c r="W41" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -3324,6 +3462,16 @@
       <c r="E42">
         <v>1.23</v>
       </c>
+      <c r="F42">
+        <v>85</v>
+      </c>
+      <c r="G42">
+        <v>3390.66</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
       <c r="I42">
         <v>86</v>
       </c>
@@ -3331,7 +3479,7 @@
         <v>950.77</v>
       </c>
       <c r="K42" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L42">
@@ -3341,7 +3489,7 @@
         <v>2935.53</v>
       </c>
       <c r="N42" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O42">
@@ -3351,7 +3499,7 @@
         <v>2435.9299999999998</v>
       </c>
       <c r="Q42" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="R42">
@@ -3361,7 +3509,7 @@
         <v>2487.52</v>
       </c>
       <c r="T42" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U42">
@@ -3371,7 +3519,7 @@
         <v>1500.97</v>
       </c>
       <c r="W42" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -3391,6 +3539,16 @@
       <c r="E43">
         <v>0.31</v>
       </c>
+      <c r="F43">
+        <v>47</v>
+      </c>
+      <c r="G43">
+        <v>7.13</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="9"/>
+        <v>opt</v>
+      </c>
       <c r="I43">
         <v>47</v>
       </c>
@@ -3398,7 +3556,7 @@
         <v>5.31</v>
       </c>
       <c r="K43" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>opt</v>
       </c>
       <c r="L43">
@@ -3408,7 +3566,7 @@
         <v>21.42</v>
       </c>
       <c r="N43" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>opt</v>
       </c>
       <c r="O43">
@@ -3418,7 +3576,7 @@
         <v>13.01</v>
       </c>
       <c r="Q43" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>opt</v>
       </c>
       <c r="R43">
@@ -3428,7 +3586,7 @@
         <v>162.75</v>
       </c>
       <c r="T43" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>opt</v>
       </c>
       <c r="U43">
@@ -3438,7 +3596,7 @@
         <v>551.9</v>
       </c>
       <c r="W43" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -3458,6 +3616,16 @@
       <c r="E44">
         <v>0.88</v>
       </c>
+      <c r="F44">
+        <v>61</v>
+      </c>
+      <c r="G44">
+        <v>3070.27</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
       <c r="I44">
         <v>63</v>
       </c>
@@ -3465,7 +3633,7 @@
         <v>31.04</v>
       </c>
       <c r="K44" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L44">
@@ -3475,7 +3643,7 @@
         <v>348.49</v>
       </c>
       <c r="N44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O44">
@@ -3485,7 +3653,7 @@
         <v>3516.79</v>
       </c>
       <c r="Q44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="R44">
@@ -3495,7 +3663,7 @@
         <v>3060.12</v>
       </c>
       <c r="T44" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U44">
@@ -3505,7 +3673,7 @@
         <v>1302.26</v>
       </c>
       <c r="W44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -3525,6 +3693,16 @@
       <c r="E45">
         <v>1.77</v>
       </c>
+      <c r="F45">
+        <v>85</v>
+      </c>
+      <c r="G45">
+        <v>541.58000000000004</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
       <c r="I45">
         <v>84</v>
       </c>
@@ -3532,7 +3710,7 @@
         <v>1204.01</v>
       </c>
       <c r="K45" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L45">
@@ -3542,7 +3720,7 @@
         <v>160.27000000000001</v>
       </c>
       <c r="N45" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O45">
@@ -3552,7 +3730,7 @@
         <v>2140.17</v>
       </c>
       <c r="Q45" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="R45">
@@ -3562,7 +3740,7 @@
         <v>2247.27</v>
       </c>
       <c r="T45" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U45">
@@ -3572,12 +3750,12 @@
         <v>2549.39</v>
       </c>
       <c r="W45" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B46">
@@ -3592,6 +3770,16 @@
       <c r="E46">
         <v>0.45</v>
       </c>
+      <c r="F46">
+        <v>49</v>
+      </c>
+      <c r="G46">
+        <v>1797.56</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="9"/>
+        <v>opt</v>
+      </c>
       <c r="I46">
         <v>51</v>
       </c>
@@ -3599,7 +3787,7 @@
         <v>30.79</v>
       </c>
       <c r="K46" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L46">
@@ -3609,7 +3797,7 @@
         <v>2167.62</v>
       </c>
       <c r="N46" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O46">
@@ -3619,7 +3807,7 @@
         <v>3148.79</v>
       </c>
       <c r="Q46" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="R46">
@@ -3629,7 +3817,7 @@
         <v>2009.49</v>
       </c>
       <c r="T46" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U46">
@@ -3639,7 +3827,7 @@
         <v>162.55000000000001</v>
       </c>
       <c r="W46" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -3659,6 +3847,16 @@
       <c r="E47">
         <v>2.54</v>
       </c>
+      <c r="F47">
+        <v>73</v>
+      </c>
+      <c r="G47">
+        <v>220.51</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="9"/>
+        <v>opt</v>
+      </c>
       <c r="I47">
         <v>73</v>
       </c>
@@ -3666,7 +3864,7 @@
         <v>274.13</v>
       </c>
       <c r="K47" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>opt</v>
       </c>
       <c r="L47">
@@ -3676,7 +3874,7 @@
         <v>3294.1</v>
       </c>
       <c r="N47" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>opt</v>
       </c>
       <c r="O47">
@@ -3686,7 +3884,7 @@
         <v>248.24</v>
       </c>
       <c r="Q47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>opt</v>
       </c>
       <c r="R47">
@@ -3696,7 +3894,7 @@
         <v>3003.53</v>
       </c>
       <c r="T47" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U47">
@@ -3706,12 +3904,12 @@
         <v>468.54</v>
       </c>
       <c r="W47" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B48">
@@ -3726,6 +3924,16 @@
       <c r="E48">
         <v>1.35</v>
       </c>
+      <c r="F48">
+        <v>68</v>
+      </c>
+      <c r="G48">
+        <v>18.3</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="9"/>
+        <v>opt</v>
+      </c>
       <c r="I48">
         <v>68</v>
       </c>
@@ -3733,7 +3941,7 @@
         <v>33.49</v>
       </c>
       <c r="K48" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>opt</v>
       </c>
       <c r="L48">
@@ -3743,7 +3951,7 @@
         <v>21.14</v>
       </c>
       <c r="N48" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O48">
@@ -3753,7 +3961,7 @@
         <v>32.380000000000003</v>
       </c>
       <c r="Q48" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>opt</v>
       </c>
       <c r="R48">
@@ -3763,7 +3971,7 @@
         <v>501.68</v>
       </c>
       <c r="T48" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="U48">
@@ -3773,7 +3981,7 @@
         <v>1847.68</v>
       </c>
       <c r="W48" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>opt</v>
       </c>
     </row>
@@ -3786,26 +3994,35 @@
         <v>70.45</v>
       </c>
       <c r="C49" s="1">
-        <f t="shared" ref="C49" si="14">AVERAGE(C29:C48)</f>
+        <f t="shared" ref="C49" si="15">AVERAGE(C29:C48)</f>
         <v>70.45</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" ref="D49" si="15">AVERAGE(D29:D48)</f>
+        <f t="shared" ref="D49" si="16">AVERAGE(D29:D48)</f>
         <v>1</v>
       </c>
       <c r="E49" s="1">
-        <f t="shared" ref="E49:P49" si="16">AVERAGE(E29:E48)</f>
+        <f t="shared" ref="E49:P49" si="17">AVERAGE(E29:E48)</f>
         <v>2.9030000000000005</v>
       </c>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
+      <c r="F49" s="1">
+        <f t="shared" si="17"/>
+        <v>71.099999999999994</v>
+      </c>
+      <c r="G49" s="1">
+        <f t="shared" si="17"/>
+        <v>1222.4570000000001</v>
+      </c>
+      <c r="H49" s="1">
+        <f>COUNTIF(H29:H48, "opt")</f>
+        <v>11</v>
+      </c>
       <c r="I49" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>71.95</v>
       </c>
       <c r="J49" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>928.15500000000009</v>
       </c>
       <c r="K49" s="1">
@@ -3813,11 +4030,11 @@
         <v>4</v>
       </c>
       <c r="L49" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>72.849999999999994</v>
       </c>
       <c r="M49" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1487.6964999999998</v>
       </c>
       <c r="N49" s="1">
@@ -3825,11 +4042,11 @@
         <v>2</v>
       </c>
       <c r="O49" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>72.3</v>
       </c>
       <c r="P49" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1466.5520000000001</v>
       </c>
       <c r="Q49" s="1">
@@ -3837,11 +4054,11 @@
         <v>3</v>
       </c>
       <c r="R49" s="1">
-        <f t="shared" ref="R49" si="17">AVERAGE(R29:R48)</f>
+        <f t="shared" ref="R49" si="18">AVERAGE(R29:R48)</f>
         <v>77.599999999999994</v>
       </c>
       <c r="S49" s="1">
-        <f t="shared" ref="S49" si="18">AVERAGE(S29:S48)</f>
+        <f t="shared" ref="S49" si="19">AVERAGE(S29:S48)</f>
         <v>2184.5685000000003</v>
       </c>
       <c r="T49" s="1">
@@ -3849,11 +4066,11 @@
         <v>1</v>
       </c>
       <c r="U49" s="1">
-        <f t="shared" ref="U49" si="19">AVERAGE(U29:U48)</f>
+        <f t="shared" ref="U49" si="20">AVERAGE(U29:U48)</f>
         <v>77.5</v>
       </c>
       <c r="V49" s="1">
-        <f t="shared" ref="V49" si="20">AVERAGE(V29:V48)</f>
+        <f t="shared" ref="V49" si="21">AVERAGE(V29:V48)</f>
         <v>1928.9090000000001</v>
       </c>
       <c r="W49" s="1">
@@ -3899,9 +4116,11 @@
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
+      <c r="F52" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
@@ -3942,9 +4161,15 @@
       <c r="E53" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
+      <c r="F53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
@@ -3986,7 +4211,7 @@
       </c>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B54">
@@ -4001,6 +4226,16 @@
       <c r="E54">
         <v>3608.26</v>
       </c>
+      <c r="F54">
+        <v>139</v>
+      </c>
+      <c r="G54">
+        <v>1127.6600000000001</v>
+      </c>
+      <c r="H54" t="str">
+        <f>IF($B54=F54, "opt", "")</f>
+        <v>opt</v>
+      </c>
       <c r="L54">
         <v>144</v>
       </c>
@@ -4058,6 +4293,16 @@
       <c r="E55">
         <v>1985.8</v>
       </c>
+      <c r="F55">
+        <v>149</v>
+      </c>
+      <c r="G55">
+        <v>1195.83</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" ref="H55:H73" si="22">IF($B55=F55, "opt", "")</f>
+        <v/>
+      </c>
       <c r="L55">
         <v>154</v>
       </c>
@@ -4065,7 +4310,7 @@
         <v>2386.46</v>
       </c>
       <c r="N55" t="str">
-        <f t="shared" ref="N55:N73" si="21">IF($B55=L55, "opt", "")</f>
+        <f t="shared" ref="N55:N73" si="23">IF($B55=L55, "opt", "")</f>
         <v/>
       </c>
       <c r="O55">
@@ -4075,7 +4320,7 @@
         <v>2672.73</v>
       </c>
       <c r="Q55" t="str">
-        <f t="shared" ref="Q55:Q73" si="22">IF($B55=O55, "opt", "")</f>
+        <f t="shared" ref="Q55:Q73" si="24">IF($B55=O55, "opt", "")</f>
         <v/>
       </c>
       <c r="R55">
@@ -4085,7 +4330,7 @@
         <v>3637.73</v>
       </c>
       <c r="T55" t="str">
-        <f t="shared" ref="T55:T73" si="23">IF($B55=R55, "opt", "")</f>
+        <f t="shared" ref="T55:T73" si="25">IF($B55=R55, "opt", "")</f>
         <v/>
       </c>
       <c r="U55">
@@ -4095,7 +4340,7 @@
         <v>2837.51</v>
       </c>
       <c r="W55" t="str">
-        <f t="shared" ref="W55:W73" si="24">IF($B55=U55, "opt", "")</f>
+        <f t="shared" ref="W55:W73" si="26">IF($B55=U55, "opt", "")</f>
         <v/>
       </c>
     </row>
@@ -4115,6 +4360,16 @@
       <c r="E56">
         <v>179.16</v>
       </c>
+      <c r="F56">
+        <v>78</v>
+      </c>
+      <c r="G56">
+        <v>183.53</v>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L56">
         <v>83</v>
       </c>
@@ -4122,7 +4377,7 @@
         <v>309.95999999999998</v>
       </c>
       <c r="N56" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O56">
@@ -4132,7 +4387,7 @@
         <v>1015.5</v>
       </c>
       <c r="Q56" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R56">
@@ -4142,7 +4397,7 @@
         <v>714.64</v>
       </c>
       <c r="T56" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U56">
@@ -4152,7 +4407,7 @@
         <v>3470.98</v>
       </c>
       <c r="W56" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -4172,6 +4427,16 @@
       <c r="E57">
         <v>3631.76</v>
       </c>
+      <c r="F57">
+        <v>148</v>
+      </c>
+      <c r="G57">
+        <v>2908.23</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L57">
         <v>154</v>
       </c>
@@ -4179,7 +4444,7 @@
         <v>2378.6999999999998</v>
       </c>
       <c r="N57" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O57">
@@ -4189,7 +4454,7 @@
         <v>1923.96</v>
       </c>
       <c r="Q57" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R57">
@@ -4199,7 +4464,7 @@
         <v>3447.42</v>
       </c>
       <c r="T57" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U57">
@@ -4209,7 +4474,7 @@
         <v>1616.56</v>
       </c>
       <c r="W57" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -4229,6 +4494,16 @@
       <c r="E58">
         <v>911.98</v>
       </c>
+      <c r="F58">
+        <v>159</v>
+      </c>
+      <c r="G58">
+        <v>624.89</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L58">
         <v>165</v>
       </c>
@@ -4236,7 +4511,7 @@
         <v>648.26</v>
       </c>
       <c r="N58" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O58">
@@ -4246,7 +4521,7 @@
         <v>2621.15</v>
       </c>
       <c r="Q58" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R58">
@@ -4256,7 +4531,7 @@
         <v>1174.47</v>
       </c>
       <c r="T58" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U58">
@@ -4266,7 +4541,7 @@
         <v>2670.1</v>
       </c>
       <c r="W58" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -4286,6 +4561,16 @@
       <c r="E59">
         <v>3604.64</v>
       </c>
+      <c r="F59">
+        <v>149</v>
+      </c>
+      <c r="G59">
+        <v>1622.87</v>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L59">
         <v>154</v>
       </c>
@@ -4293,7 +4578,7 @@
         <v>1211.22</v>
       </c>
       <c r="N59" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O59">
@@ -4303,7 +4588,7 @@
         <v>1347.62</v>
       </c>
       <c r="Q59" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R59">
@@ -4313,7 +4598,7 @@
         <v>1435.66</v>
       </c>
       <c r="T59" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U59">
@@ -4323,7 +4608,7 @@
         <v>3351.26</v>
       </c>
       <c r="W59" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -4343,6 +4628,16 @@
       <c r="E60">
         <v>3655.54</v>
       </c>
+      <c r="F60">
+        <v>157</v>
+      </c>
+      <c r="G60">
+        <v>1349.34</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L60">
         <v>162</v>
       </c>
@@ -4350,7 +4645,7 @@
         <v>1868.42</v>
       </c>
       <c r="N60" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O60">
@@ -4360,7 +4655,7 @@
         <v>1825.03</v>
       </c>
       <c r="Q60" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R60">
@@ -4370,7 +4665,7 @@
         <v>1391.51</v>
       </c>
       <c r="T60" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U60">
@@ -4380,7 +4675,7 @@
         <v>2752.16</v>
       </c>
       <c r="W60" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -4400,6 +4695,16 @@
       <c r="E61">
         <v>3648.06</v>
       </c>
+      <c r="F61">
+        <v>176</v>
+      </c>
+      <c r="G61">
+        <v>1061.81</v>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L61">
         <v>177</v>
       </c>
@@ -4407,7 +4712,7 @@
         <v>3139.32</v>
       </c>
       <c r="N61" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O61">
@@ -4417,7 +4722,7 @@
         <v>2940.9</v>
       </c>
       <c r="Q61" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R61">
@@ -4427,7 +4732,7 @@
         <v>1329.91</v>
       </c>
       <c r="T61" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U61">
@@ -4437,7 +4742,7 @@
         <v>1546.74</v>
       </c>
       <c r="W61" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -4457,6 +4762,16 @@
       <c r="E62">
         <v>329.38</v>
       </c>
+      <c r="F62">
+        <v>153</v>
+      </c>
+      <c r="G62">
+        <v>1347.81</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L62">
         <v>156</v>
       </c>
@@ -4464,7 +4779,7 @@
         <v>1556.14</v>
       </c>
       <c r="N62" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O62">
@@ -4474,7 +4789,7 @@
         <v>1724.02</v>
       </c>
       <c r="Q62" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R62">
@@ -4484,7 +4799,7 @@
         <v>3240.09</v>
       </c>
       <c r="T62" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U62">
@@ -4494,7 +4809,7 @@
         <v>3490.77</v>
       </c>
       <c r="W62" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -4514,6 +4829,16 @@
       <c r="E63">
         <v>3602.38</v>
       </c>
+      <c r="F63">
+        <v>149</v>
+      </c>
+      <c r="G63">
+        <v>1544.1</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L63">
         <v>153</v>
       </c>
@@ -4521,7 +4846,7 @@
         <v>3116.66</v>
       </c>
       <c r="N63" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O63">
@@ -4531,7 +4856,7 @@
         <v>1856.66</v>
       </c>
       <c r="Q63" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R63">
@@ -4541,7 +4866,7 @@
         <v>3571.87</v>
       </c>
       <c r="T63" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U63">
@@ -4551,7 +4876,7 @@
         <v>2597.0500000000002</v>
       </c>
       <c r="W63" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -4571,6 +4896,16 @@
       <c r="E64">
         <v>338.36</v>
       </c>
+      <c r="F64">
+        <v>113</v>
+      </c>
+      <c r="G64">
+        <v>2530.9</v>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L64">
         <v>117</v>
       </c>
@@ -4578,7 +4913,7 @@
         <v>1565.52</v>
       </c>
       <c r="N64" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O64">
@@ -4588,7 +4923,7 @@
         <v>2136.59</v>
       </c>
       <c r="Q64" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R64">
@@ -4598,7 +4933,7 @@
         <v>2636.94</v>
       </c>
       <c r="T64" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U64">
@@ -4608,7 +4943,7 @@
         <v>3155.58</v>
       </c>
       <c r="W64" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -4628,6 +4963,16 @@
       <c r="E65">
         <v>3620.36</v>
       </c>
+      <c r="F65">
+        <v>156</v>
+      </c>
+      <c r="G65">
+        <v>1474.89</v>
+      </c>
+      <c r="H65" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L65">
         <v>162</v>
       </c>
@@ -4635,7 +4980,7 @@
         <v>882.17</v>
       </c>
       <c r="N65" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O65">
@@ -4645,7 +4990,7 @@
         <v>956.97</v>
       </c>
       <c r="Q65" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R65">
@@ -4655,7 +5000,7 @@
         <v>5236.25</v>
       </c>
       <c r="T65" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U65">
@@ -4665,7 +5010,7 @@
         <v>3430.55</v>
       </c>
       <c r="W65" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -4685,6 +5030,16 @@
       <c r="E66">
         <v>913.1</v>
       </c>
+      <c r="F66">
+        <v>152</v>
+      </c>
+      <c r="G66">
+        <v>1319.81</v>
+      </c>
+      <c r="H66" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L66">
         <v>156</v>
       </c>
@@ -4692,7 +5047,7 @@
         <v>3508.34</v>
       </c>
       <c r="N66" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O66">
@@ -4702,7 +5057,7 @@
         <v>2765.03</v>
       </c>
       <c r="Q66" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R66">
@@ -4712,7 +5067,7 @@
         <v>1399.34</v>
       </c>
       <c r="T66" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U66">
@@ -4722,7 +5077,7 @@
         <v>2690.94</v>
       </c>
       <c r="W66" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -4742,6 +5097,16 @@
       <c r="E67">
         <v>236.64</v>
       </c>
+      <c r="F67">
+        <v>166</v>
+      </c>
+      <c r="G67">
+        <v>1197.1400000000001</v>
+      </c>
+      <c r="H67" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L67">
         <v>172</v>
       </c>
@@ -4749,7 +5114,7 @@
         <v>1535.47</v>
       </c>
       <c r="N67" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O67">
@@ -4759,7 +5124,7 @@
         <v>3493.09</v>
       </c>
       <c r="Q67" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R67">
@@ -4769,7 +5134,7 @@
         <v>3558.47</v>
       </c>
       <c r="T67" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U67">
@@ -4779,12 +5144,12 @@
         <v>1410.68</v>
       </c>
       <c r="W67" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B68">
@@ -4799,6 +5164,16 @@
       <c r="E68">
         <v>17.079999999999998</v>
       </c>
+      <c r="F68">
+        <v>89</v>
+      </c>
+      <c r="G68">
+        <v>271.16000000000003</v>
+      </c>
+      <c r="H68" t="str">
+        <f t="shared" si="22"/>
+        <v>opt</v>
+      </c>
       <c r="L68">
         <v>89</v>
       </c>
@@ -4806,7 +5181,7 @@
         <v>1872.38</v>
       </c>
       <c r="N68" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>opt</v>
       </c>
       <c r="O68">
@@ -4816,7 +5191,7 @@
         <v>20.65</v>
       </c>
       <c r="Q68" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R68">
@@ -4826,7 +5201,7 @@
         <v>2570.6</v>
       </c>
       <c r="T68" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U68">
@@ -4836,7 +5211,7 @@
         <v>894.18</v>
       </c>
       <c r="W68" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -4856,6 +5231,16 @@
       <c r="E69">
         <v>227.07</v>
       </c>
+      <c r="F69">
+        <v>116</v>
+      </c>
+      <c r="G69">
+        <v>1001.59</v>
+      </c>
+      <c r="H69" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L69">
         <v>121</v>
       </c>
@@ -4863,7 +5248,7 @@
         <v>1535.21</v>
       </c>
       <c r="N69" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O69">
@@ -4873,7 +5258,7 @@
         <v>3062.52</v>
       </c>
       <c r="Q69" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R69">
@@ -4883,7 +5268,7 @@
         <v>2018.32</v>
       </c>
       <c r="T69" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U69">
@@ -4893,7 +5278,7 @@
         <v>3492.04</v>
       </c>
       <c r="W69" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -4913,6 +5298,16 @@
       <c r="E70">
         <v>3650.96</v>
       </c>
+      <c r="F70">
+        <v>161</v>
+      </c>
+      <c r="G70">
+        <v>899.57</v>
+      </c>
+      <c r="H70" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L70">
         <v>166</v>
       </c>
@@ -4920,7 +5315,7 @@
         <v>3144.44</v>
       </c>
       <c r="N70" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O70">
@@ -4930,7 +5325,7 @@
         <v>1031.4100000000001</v>
       </c>
       <c r="Q70" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R70">
@@ -4940,7 +5335,7 @@
         <v>2915.07</v>
       </c>
       <c r="T70" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U70">
@@ -4950,7 +5345,7 @@
         <v>2578.83</v>
       </c>
       <c r="W70" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -4970,6 +5365,16 @@
       <c r="E71">
         <v>53.23</v>
       </c>
+      <c r="F71">
+        <v>98</v>
+      </c>
+      <c r="G71">
+        <v>502.15</v>
+      </c>
+      <c r="H71" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L71">
         <v>99</v>
       </c>
@@ -4977,7 +5382,7 @@
         <v>1565.23</v>
       </c>
       <c r="N71" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O71">
@@ -4987,7 +5392,7 @@
         <v>351.49</v>
       </c>
       <c r="Q71" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R71">
@@ -4997,7 +5402,7 @@
         <v>891.9</v>
       </c>
       <c r="T71" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U71">
@@ -5007,7 +5412,7 @@
         <v>1374.47</v>
       </c>
       <c r="W71" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -5027,6 +5432,16 @@
       <c r="E72">
         <v>3637.62</v>
       </c>
+      <c r="F72">
+        <v>141</v>
+      </c>
+      <c r="G72">
+        <v>2469.15</v>
+      </c>
+      <c r="H72" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L72">
         <v>144</v>
       </c>
@@ -5034,7 +5449,7 @@
         <v>927.05</v>
       </c>
       <c r="N72" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O72">
@@ -5044,7 +5459,7 @@
         <v>903.06</v>
       </c>
       <c r="Q72" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R72">
@@ -5054,7 +5469,7 @@
         <v>1895.86</v>
       </c>
       <c r="T72" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U72">
@@ -5064,7 +5479,7 @@
         <v>3455.11</v>
       </c>
       <c r="W72" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -5084,6 +5499,16 @@
       <c r="E73">
         <v>31.71</v>
       </c>
+      <c r="F73">
+        <v>131</v>
+      </c>
+      <c r="G73">
+        <v>442.44</v>
+      </c>
+      <c r="H73" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
       <c r="L73">
         <v>132</v>
       </c>
@@ -5091,7 +5516,7 @@
         <v>2536.19</v>
       </c>
       <c r="N73" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O73">
@@ -5101,7 +5526,7 @@
         <v>2013.01</v>
       </c>
       <c r="Q73" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R73">
@@ -5111,7 +5536,7 @@
         <v>1693.27</v>
       </c>
       <c r="T73" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="U73">
@@ -5121,7 +5546,7 @@
         <v>1350.2</v>
       </c>
       <c r="W73" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -5134,29 +5559,38 @@
         <v>136.05000000000001</v>
       </c>
       <c r="C74" s="1">
-        <f t="shared" ref="C74" si="25">AVERAGE(C54:C73)</f>
+        <f t="shared" ref="C74" si="27">AVERAGE(C54:C73)</f>
         <v>135.35</v>
       </c>
       <c r="D74" s="1">
-        <f t="shared" ref="D74" si="26">AVERAGE(D54:D73)</f>
+        <f t="shared" ref="D74" si="28">AVERAGE(D54:D73)</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="E74" s="1">
-        <f t="shared" ref="E74:P74" si="27">AVERAGE(E54:E73)</f>
+        <f t="shared" ref="E74:P74" si="29">AVERAGE(E54:E73)</f>
         <v>1894.1545000000006</v>
       </c>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
+      <c r="F74" s="1">
+        <f t="shared" si="29"/>
+        <v>139</v>
+      </c>
+      <c r="G74" s="1">
+        <f t="shared" si="29"/>
+        <v>1253.7435</v>
+      </c>
+      <c r="H74" s="1">
+        <f>COUNTIF(H54:H73, "opt")</f>
+        <v>2</v>
+      </c>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>143</v>
       </c>
       <c r="M74" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>1797.086</v>
       </c>
       <c r="N74" s="1">
@@ -5164,11 +5598,11 @@
         <v>1</v>
       </c>
       <c r="O74" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>142.15</v>
       </c>
       <c r="P74" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>1765.9225000000001</v>
       </c>
       <c r="Q74" s="1">
@@ -5176,11 +5610,11 @@
         <v>0</v>
       </c>
       <c r="R74" s="1">
-        <f t="shared" ref="R74" si="28">AVERAGE(R54:R73)</f>
+        <f t="shared" ref="R74" si="30">AVERAGE(R54:R73)</f>
         <v>154.85</v>
       </c>
       <c r="S74" s="1">
-        <f t="shared" ref="S74" si="29">AVERAGE(S54:S73)</f>
+        <f t="shared" ref="S74" si="31">AVERAGE(S54:S73)</f>
         <v>2269.5409999999997</v>
       </c>
       <c r="T74" s="1">
@@ -5188,11 +5622,11 @@
         <v>0</v>
       </c>
       <c r="U74" s="1">
-        <f t="shared" ref="U74" si="30">AVERAGE(U54:U73)</f>
+        <f t="shared" ref="U74" si="32">AVERAGE(U54:U73)</f>
         <v>150.6</v>
       </c>
       <c r="V74" s="1">
-        <f t="shared" ref="V74" si="31">AVERAGE(V54:V73)</f>
+        <f t="shared" ref="V74" si="33">AVERAGE(V54:V73)</f>
         <v>2551.4195000000004</v>
       </c>
       <c r="W74" s="1">
@@ -5201,10 +5635,10 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Y1:AA20">
-    <sortCondition ref="Y1:Y20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Y1:AA74">
+    <sortCondition ref="Y1:Y74"/>
   </sortState>
-  <mergeCells count="21">
+  <mergeCells count="23">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="U2:W2"/>
@@ -5226,6 +5660,8 @@
     <mergeCell ref="L27:N27"/>
     <mergeCell ref="L52:N52"/>
     <mergeCell ref="I27:K27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F52:H52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Testing alg. with GA params.
</commit_message>
<xml_diff>
--- a/algorithms/results/comparison.xlsx
+++ b/algorithms/results/comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\akcijanje\nauka\moji radovi\aktivno\k-domination\algorithms\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A3EE63-B034-4614-BD30-00B5D8314F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D56AC6-36E1-43E4-9F26-9FB35431C067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3555" windowWidth="29040" windowHeight="15840" xr2:uid="{9811A06C-B274-406A-BE4D-18F0FA4A89B1}"/>
   </bookViews>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C114BA-E20E-4760-908C-9E2FAA6D010C}">
   <dimension ref="A1:AG74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +743,7 @@
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4">
@@ -849,7 +849,7 @@
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5">
@@ -955,7 +955,7 @@
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6">
@@ -1061,7 +1061,7 @@
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B7">
@@ -1167,7 +1167,7 @@
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B8">
@@ -1273,7 +1273,7 @@
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9">
@@ -1379,7 +1379,7 @@
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B10">
@@ -1485,7 +1485,7 @@
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B11">
@@ -1591,7 +1591,7 @@
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12">
@@ -1697,7 +1697,7 @@
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13">
@@ -1803,7 +1803,7 @@
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14">
@@ -1909,7 +1909,7 @@
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15">
@@ -2015,7 +2015,7 @@
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16">
@@ -2121,7 +2121,7 @@
       </c>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B17">
@@ -2227,7 +2227,7 @@
       </c>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B18">
@@ -2333,7 +2333,7 @@
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B19">
@@ -2439,7 +2439,7 @@
       </c>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B20">
@@ -2545,7 +2545,7 @@
       </c>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B21">
@@ -2642,7 +2642,7 @@
       </c>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B22">
@@ -2739,7 +2739,7 @@
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B23">
@@ -3127,7 +3127,7 @@
       </c>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B29">
@@ -3224,7 +3224,7 @@
       </c>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B30">
@@ -3321,7 +3321,7 @@
       </c>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B31">
@@ -3418,7 +3418,7 @@
       </c>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B32">
@@ -3515,7 +3515,7 @@
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B33">
@@ -3612,7 +3612,7 @@
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B34">
@@ -3709,7 +3709,7 @@
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B35">
@@ -3806,7 +3806,7 @@
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B36">
@@ -3903,7 +3903,7 @@
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B37">
@@ -4000,7 +4000,7 @@
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B38">
@@ -4097,7 +4097,7 @@
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B39">
@@ -4194,7 +4194,7 @@
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B40">
@@ -4291,7 +4291,7 @@
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B41">
@@ -4388,7 +4388,7 @@
       </c>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B42">
@@ -4485,7 +4485,7 @@
       </c>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B43">
@@ -4582,7 +4582,7 @@
       </c>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B44">
@@ -4679,7 +4679,7 @@
       </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B45">
@@ -4776,7 +4776,7 @@
       </c>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B46">
@@ -4873,7 +4873,7 @@
       </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B47">
@@ -4970,7 +4970,7 @@
       </c>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B48">
@@ -7202,15 +7202,16 @@
     <sortCondition ref="AE1:AE20"/>
   </sortState>
   <mergeCells count="29">
-    <mergeCell ref="I52:K52"/>
-    <mergeCell ref="B51:AC51"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="X52:Z52"/>
-    <mergeCell ref="AA52:AC52"/>
-    <mergeCell ref="U52:W52"/>
-    <mergeCell ref="R52:T52"/>
-    <mergeCell ref="L52:N52"/>
-    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="AA2:AC2"/>
+    <mergeCell ref="B1:AC1"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F2:H2"/>
     <mergeCell ref="B26:AC26"/>
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="X27:Z27"/>
@@ -7221,16 +7222,15 @@
     <mergeCell ref="L27:N27"/>
     <mergeCell ref="I27:K27"/>
     <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="B1:AC1"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I52:K52"/>
+    <mergeCell ref="B51:AC51"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="X52:Z52"/>
+    <mergeCell ref="AA52:AC52"/>
+    <mergeCell ref="U52:W52"/>
+    <mergeCell ref="R52:T52"/>
+    <mergeCell ref="L52:N52"/>
+    <mergeCell ref="F52:H52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Initial results in tex.
</commit_message>
<xml_diff>
--- a/algorithms/results/comparison.xlsx
+++ b/algorithms/results/comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\akcijanje\nauka\moji radovi\aktivno\k-domination\algorithms\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E15D012-707E-4C26-B0A5-EAD0C4CFAE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8557385E-6F16-4B7F-90B9-A4D7AFF0941A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3555" windowWidth="29040" windowHeight="15840" xr2:uid="{9811A06C-B274-406A-BE4D-18F0FA4A89B1}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="77">
   <si>
     <t>bath.txt</t>
   </si>
@@ -189,6 +189,87 @@
   </si>
   <si>
     <t>SG</t>
+  </si>
+  <si>
+    <t>Bath</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Brighton</t>
+  </si>
+  <si>
+    <t>Bristol</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>Coventry</t>
+  </si>
+  <si>
+    <t>Exeter</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>Leeds</t>
+  </si>
+  <si>
+    <t>Leicester</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Newcastle</t>
+  </si>
+  <si>
+    <t>Nottingham</t>
+  </si>
+  <si>
+    <t>Oxford</t>
+  </si>
+  <si>
+    <t>Plymouth</t>
+  </si>
+  <si>
+    <t>Sheffield</t>
+  </si>
+  <si>
+    <t>Southampton</t>
+  </si>
+  <si>
+    <t>Sunderland</t>
+  </si>
+  <si>
+    <t>York</t>
+  </si>
+  <si>
+    <t>Belgrade</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Dublin</t>
+  </si>
+  <si>
+    <t>Minsk</t>
+  </si>
+  <si>
+    <t>\hline</t>
+  </si>
+  <si>
+    <t>City &amp; Best &amp; Avg. &amp; T &amp; Alg. &amp; Best &amp; Avg. \\ \hline</t>
   </si>
 </sst>
 </file>
@@ -555,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C114BA-E20E-4760-908C-9E2FAA6D010C}">
-  <dimension ref="A1:N89"/>
+  <dimension ref="A1:P89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G93" sqref="G93"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P64" sqref="P64:P88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,7 +649,7 @@
     <col min="5" max="8" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -580,7 +661,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>31</v>
@@ -596,7 +677,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -639,10 +720,13 @@
       <c r="N3" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B4">
         <v>38</v>
@@ -689,10 +773,14 @@
       <c r="N4">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P4" t="str">
+        <f>A4&amp;"&amp;"&amp;IF(E4&lt;=L4,"\bf{"&amp;E4&amp;"}",E4)&amp;"&amp;"&amp;ROUND(G4,1)&amp;"&amp;"&amp;ROUND(J4,1)&amp;"&amp;"&amp;K4&amp;"&amp;"&amp;IF(L4&lt;=E4,"\bf{"&amp;L4&amp;"}",L4)&amp;"&amp;"&amp;ROUND(M4,1)&amp;"\\"</f>
+        <v>Bath&amp;\bf{38}&amp;38&amp;445.5&amp;BS4&amp;43&amp;44.6\\</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="B5">
         <v>39</v>
@@ -739,10 +827,14 @@
       <c r="N5">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P5" t="str">
+        <f t="shared" ref="P5:P28" si="1">A5&amp;"&amp;"&amp;IF(E5&lt;=L5,"\bf{"&amp;E5&amp;"}",E5)&amp;"&amp;"&amp;ROUND(G5,1)&amp;"&amp;"&amp;ROUND(J5,1)&amp;"&amp;"&amp;K5&amp;"&amp;"&amp;IF(L5&lt;=E5,"\bf{"&amp;L5&amp;"}",L5)&amp;"&amp;"&amp;ROUND(M5,1)&amp;"\\"</f>
+        <v>Belfast&amp;\bf{39}&amp;39&amp;838.3&amp;BS4&amp;48&amp;50.2\\</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="B6">
         <v>21</v>
@@ -789,10 +881,14 @@
       <c r="N6">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P6" t="str">
+        <f t="shared" si="1"/>
+        <v>Brighton&amp;\bf{21}&amp;21&amp;463.4&amp;BS4&amp;28&amp;28.2\\</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>37</v>
@@ -839,10 +935,14 @@
       <c r="N7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P7" t="str">
+        <f t="shared" si="1"/>
+        <v>Bristol&amp;\bf{37}&amp;37&amp;791.3&amp;BS2&amp;46&amp;47.4\\</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B8">
         <v>39</v>
@@ -889,10 +989,14 @@
       <c r="N8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P8" t="str">
+        <f t="shared" si="1"/>
+        <v>Cardiff&amp;\bf{39}&amp;39&amp;419.5&amp;BS4&amp;48&amp;50.6\\</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="B9">
         <v>38</v>
@@ -939,10 +1043,14 @@
       <c r="N9">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P9" t="str">
+        <f t="shared" si="1"/>
+        <v>Coventry&amp;\bf{38}&amp;38.2&amp;438.4&amp;BS4&amp;170&amp;172.6\\</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B10">
         <v>38</v>
@@ -989,10 +1097,14 @@
       <c r="N10">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P10" t="str">
+        <f t="shared" si="1"/>
+        <v>Exeter&amp;\bf{38}&amp;38&amp;514.2&amp;BS4&amp;181&amp;182.3\\</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="B11">
         <v>50</v>
@@ -1039,10 +1151,14 @@
       <c r="N11">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P11" t="str">
+        <f t="shared" si="1"/>
+        <v>Glasgow&amp;\bf{50}&amp;50.2&amp;416&amp;BS4&amp;197&amp;199.8\\</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B12">
         <v>40</v>
@@ -1089,10 +1205,14 @@
       <c r="N12">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P12" t="str">
+        <f t="shared" si="1"/>
+        <v>Leeds&amp;\bf{40}&amp;40&amp;685.6&amp;BS4&amp;186&amp;187.1\\</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B13">
         <v>38</v>
@@ -1139,10 +1259,14 @@
       <c r="N13">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P13" t="str">
+        <f t="shared" si="1"/>
+        <v>Leicester&amp;\bf{38}&amp;38&amp;1010.4&amp;BS4&amp;175&amp;177.7\\</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="B14">
         <v>28</v>
@@ -1189,10 +1313,14 @@
       <c r="N14">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P14" t="str">
+        <f t="shared" si="1"/>
+        <v>Liverpool&amp;\bf{28}&amp;28&amp;700.5&amp;BS4&amp;132&amp;133\\</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="B15">
         <v>38</v>
@@ -1239,10 +1367,14 @@
       <c r="N15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P15" t="str">
+        <f t="shared" si="1"/>
+        <v>Manchester&amp;\bf{38}&amp;38.8&amp;2071.7&amp;BS4&amp;177&amp;178.5\\</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="B16">
         <v>44</v>
@@ -1289,10 +1421,14 @@
       <c r="N16">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P16" t="str">
+        <f t="shared" si="1"/>
+        <v>Newcastle&amp;\bf{44}&amp;44&amp;611.7&amp;BS2&amp;169&amp;171.5\\</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B17">
         <v>44</v>
@@ -1339,10 +1475,14 @@
       <c r="N17">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P17" t="str">
+        <f t="shared" si="1"/>
+        <v>Nottingham&amp;\bf{44}&amp;44&amp;1211&amp;BS4&amp;193&amp;195.2\\</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="B18">
         <v>24</v>
@@ -1389,10 +1529,14 @@
       <c r="N18">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P18" t="str">
+        <f t="shared" si="1"/>
+        <v>Oxford&amp;\bf{24}&amp;24&amp;63.1&amp;BS2&amp;99&amp;100.8\\</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B19">
         <v>31</v>
@@ -1439,10 +1583,14 @@
       <c r="N19">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P19" t="str">
+        <f t="shared" si="1"/>
+        <v>Plymouth&amp;\bf{31}&amp;31&amp;707.2&amp;BS4&amp;135&amp;137\\</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B20">
         <v>42</v>
@@ -1489,10 +1637,14 @@
       <c r="N20">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P20" t="str">
+        <f t="shared" si="1"/>
+        <v>Sheffield&amp;\bf{42}&amp;42&amp;878.2&amp;BS4&amp;180&amp;182.2\\</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B21">
         <v>25</v>
@@ -1539,10 +1691,14 @@
       <c r="N21">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P21" t="str">
+        <f t="shared" si="1"/>
+        <v>Southampton&amp;\bf{25}&amp;25&amp;277.5&amp;BS4&amp;112&amp;113.2\\</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="B22">
         <v>36</v>
@@ -1589,10 +1745,14 @@
       <c r="N22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P22" t="str">
+        <f t="shared" si="1"/>
+        <v>Sunderland&amp;\bf{36}&amp;36&amp;688.6&amp;BS4&amp;162&amp;163.6\\</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="B23">
         <v>32</v>
@@ -1639,10 +1799,14 @@
       <c r="N23">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P23" t="str">
+        <f t="shared" si="1"/>
+        <v>York&amp;\bf{32}&amp;32&amp;324.6&amp;BS4&amp;144&amp;145.8\\</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="E24">
         <f>MIN('k1'!B23,'k1'!F23,'k1'!J23,'k1'!N23,'k1'!R23,'k1'!V23,'k1'!Z23,'k1'!AD23,'k1'!AH23,'k1'!AL23)</f>
@@ -1680,10 +1844,14 @@
       <c r="N24">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P24" t="str">
+        <f t="shared" si="1"/>
+        <v>Belgrade&amp;\bf{85}&amp;88.7&amp;3610.8&amp;PG&amp;99&amp;100.3\\</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="E25">
         <f>MIN('k1'!B24,'k1'!F24,'k1'!J24,'k1'!N24,'k1'!R24,'k1'!V24,'k1'!Z24,'k1'!AD24,'k1'!AH24,'k1'!AL24)</f>
@@ -1721,10 +1889,14 @@
       <c r="N25">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P25" t="str">
+        <f t="shared" si="1"/>
+        <v>Berlin&amp;\bf{102}&amp;104.7&amp;3609.5&amp;SG&amp;146&amp;147\\</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="E26">
         <f>MIN('k1'!B25,'k1'!F25,'k1'!J25,'k1'!N25,'k1'!R25,'k1'!V25,'k1'!Z25,'k1'!AD25,'k1'!AH25,'k1'!AL25)</f>
@@ -1762,10 +1934,14 @@
       <c r="N26">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P26" t="str">
+        <f t="shared" si="1"/>
+        <v>Boston&amp;99&amp;101.1&amp;3685.6&amp;SG&amp;\bf{71}&amp;72.6\\</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E27">
         <f>MIN('k1'!B26,'k1'!F26,'k1'!J26,'k1'!N26,'k1'!R26,'k1'!V26,'k1'!Z26,'k1'!AD26,'k1'!AH26,'k1'!AL26)</f>
@@ -1803,10 +1979,14 @@
       <c r="N27">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P27" t="str">
+        <f t="shared" si="1"/>
+        <v>Dublin&amp;96&amp;99.7&amp;3790.3&amp;PG&amp;\bf{88}&amp;90.2\\</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="E28">
         <f>MIN('k1'!B27,'k1'!F27,'k1'!J27,'k1'!N27,'k1'!R27,'k1'!V27,'k1'!Z27,'k1'!AD27,'k1'!AH27,'k1'!AL27)</f>
@@ -1844,21 +2024,25 @@
       <c r="N28">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P28" t="str">
+        <f t="shared" si="1"/>
+        <v>Minsk&amp;\bf{100}&amp;102.2&amp;3602.3&amp;SG&amp;138&amp;139.3\\</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="1">
-        <f t="shared" ref="B29:D29" si="1">AVERAGE(B4:B23)</f>
+        <f t="shared" ref="B29:D29" si="2">AVERAGE(B4:B23)</f>
         <v>36.1</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.37649999999999995</v>
       </c>
       <c r="E29" s="1">
@@ -1874,32 +2058,35 @@
         <v>48.781333333333329</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" ref="H29:L29" si="2">AVERAGE(H4:H28)</f>
+        <f t="shared" ref="H29:L29" si="3">AVERAGE(H4:H28)</f>
         <v>0.4533028710235677</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>528.7252666666667</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1274.2051777777776</v>
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>126.68</v>
       </c>
       <c r="M29" s="1">
-        <f t="shared" ref="M29" si="3">AVERAGE(M4:M28)</f>
+        <f t="shared" ref="M29" si="4">AVERAGE(M4:M28)</f>
         <v>128.428</v>
       </c>
       <c r="N29" s="1">
-        <f t="shared" ref="N29" si="4">AVERAGE(N4:N28)</f>
+        <f t="shared" ref="N29" si="5">AVERAGE(N4:N28)</f>
         <v>1.1239999999999997</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1911,7 +2098,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
         <v>31</v>
@@ -1927,7 +2114,7 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>20</v>
       </c>
@@ -1970,10 +2157,13 @@
       <c r="N33" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B34">
         <v>71</v>
@@ -2020,10 +2210,14 @@
       <c r="N34">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P34" t="str">
+        <f>A34&amp;"&amp;"&amp;IF(E34&lt;=L34,"\bf{"&amp;E34&amp;"}",E34)&amp;"&amp;"&amp;ROUND(G34,1)&amp;"&amp;"&amp;ROUND(J34,1)&amp;"&amp;"&amp;K34&amp;"&amp;"&amp;IF(L34&lt;=E34,"\bf{"&amp;L34&amp;"}",L34)&amp;"&amp;"&amp;ROUND(M34,1)&amp;"\\"</f>
+        <v>Bath&amp;\bf{71}&amp;71.8&amp;634.1&amp;BS1&amp;86&amp;89\\</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="B35">
         <v>76</v>
@@ -2039,7 +2233,7 @@
         <v>76</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" ref="F35:F58" si="5">IF(E35=$B35,"best","")</f>
+        <f t="shared" ref="F35:F58" si="6">IF(E35=$B35,"best","")</f>
         <v>best</v>
       </c>
       <c r="G35">
@@ -2070,10 +2264,14 @@
       <c r="N35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P35" t="str">
+        <f t="shared" ref="P35:P58" si="7">A35&amp;"&amp;"&amp;IF(E35&lt;=L35,"\bf{"&amp;E35&amp;"}",E35)&amp;"&amp;"&amp;ROUND(G35,1)&amp;"&amp;"&amp;ROUND(J35,1)&amp;"&amp;"&amp;K35&amp;"&amp;"&amp;IF(L35&lt;=E35,"\bf{"&amp;L35&amp;"}",L35)&amp;"&amp;"&amp;ROUND(M35,1)&amp;"\\"</f>
+        <v>Belfast&amp;\bf{76}&amp;76.2&amp;1675.3&amp;BS4&amp;96&amp;97.6\\</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="B36">
         <v>40</v>
@@ -2089,7 +2287,7 @@
         <v>40</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>best</v>
       </c>
       <c r="G36">
@@ -2120,10 +2318,14 @@
       <c r="N36">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P36" t="str">
+        <f t="shared" si="7"/>
+        <v>Brighton&amp;\bf{40}&amp;41.1&amp;574.7&amp;BS4&amp;49&amp;49.4\\</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="B37">
         <v>72</v>
@@ -2139,7 +2341,7 @@
         <v>73</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G37">
@@ -2170,10 +2372,14 @@
       <c r="N37">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P37" t="str">
+        <f t="shared" si="7"/>
+        <v>Bristol&amp;\bf{73}&amp;73.7&amp;1588.6&amp;BS4&amp;91&amp;94\\</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B38">
         <v>78</v>
@@ -2189,7 +2395,7 @@
         <v>79</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G38">
@@ -2220,10 +2426,14 @@
       <c r="N38">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P38" t="str">
+        <f t="shared" si="7"/>
+        <v>Cardiff&amp;\bf{79}&amp;79.4&amp;897&amp;BS4&amp;92&amp;95.9\\</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="B39">
         <v>72</v>
@@ -2239,7 +2449,7 @@
         <v>73</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G39">
@@ -2270,10 +2480,14 @@
       <c r="N39">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P39" t="str">
+        <f t="shared" si="7"/>
+        <v>Coventry&amp;\bf{73}&amp;73.2&amp;937.9&amp;BS4&amp;84&amp;85.1\\</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B40">
         <v>76</v>
@@ -2289,7 +2503,7 @@
         <v>77</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G40">
@@ -2320,10 +2534,14 @@
       <c r="N40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P40" t="str">
+        <f t="shared" si="7"/>
+        <v>Exeter&amp;\bf{77}&amp;77.3&amp;582.5&amp;BS4&amp;94&amp;95.7\\</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="B41">
         <v>93</v>
@@ -2339,7 +2557,7 @@
         <v>93</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>best</v>
       </c>
       <c r="G41">
@@ -2370,10 +2588,14 @@
       <c r="N41">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P41" t="str">
+        <f t="shared" si="7"/>
+        <v>Glasgow&amp;\bf{93}&amp;94.2&amp;671&amp;BS4&amp;108&amp;110.6\\</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B42">
         <v>78</v>
@@ -2389,7 +2611,7 @@
         <v>79</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G42">
@@ -2420,10 +2642,14 @@
       <c r="N42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P42" t="str">
+        <f t="shared" si="7"/>
+        <v>Leeds&amp;\bf{79}&amp;80.5&amp;815&amp;BS4&amp;98&amp;99.6\\</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B43">
         <v>75</v>
@@ -2439,7 +2665,7 @@
         <v>75</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>best</v>
       </c>
       <c r="G43">
@@ -2470,10 +2696,14 @@
       <c r="N43">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P43" t="str">
+        <f t="shared" si="7"/>
+        <v>Leicester&amp;\bf{75}&amp;75.2&amp;1056.6&amp;BS4&amp;93&amp;94.1\\</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="B44">
         <v>56</v>
@@ -2489,7 +2719,7 @@
         <v>57</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G44">
@@ -2520,10 +2750,14 @@
       <c r="N44">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P44" t="str">
+        <f t="shared" si="7"/>
+        <v>Liverpool&amp;\bf{57}&amp;57&amp;1157.7&amp;BS4&amp;71&amp;72\\</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="B45">
         <v>76</v>
@@ -2539,7 +2773,7 @@
         <v>77</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G45">
@@ -2570,10 +2804,14 @@
       <c r="N45">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P45" t="str">
+        <f t="shared" si="7"/>
+        <v>Manchester&amp;\bf{77}&amp;78.4&amp;3053.1&amp;BS4&amp;90&amp;91.5\\</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="B46">
         <v>83</v>
@@ -2589,7 +2827,7 @@
         <v>83</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>best</v>
       </c>
       <c r="G46">
@@ -2620,10 +2858,14 @@
       <c r="N46">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P46" t="str">
+        <f t="shared" si="7"/>
+        <v>Newcastle&amp;\bf{83}&amp;84.3&amp;823.1&amp;BS4&amp;94&amp;95.4\\</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B47">
         <v>83</v>
@@ -2639,7 +2881,7 @@
         <v>84</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G47">
@@ -2670,10 +2912,14 @@
       <c r="N47">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P47" t="str">
+        <f t="shared" si="7"/>
+        <v>Nottingham&amp;\bf{84}&amp;85.3&amp;2167.1&amp;BS4&amp;102&amp;103.3\\</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="B48">
         <v>47</v>
@@ -2689,7 +2935,7 @@
         <v>47</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>best</v>
       </c>
       <c r="G48">
@@ -2720,10 +2966,14 @@
       <c r="N48">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P48" t="str">
+        <f t="shared" si="7"/>
+        <v>Oxford&amp;\bf{47}&amp;47&amp;83&amp;BS4&amp;54&amp;54.9\\</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B49">
         <v>60</v>
@@ -2739,7 +2989,7 @@
         <v>62</v>
       </c>
       <c r="F49" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G49">
@@ -2770,10 +3020,14 @@
       <c r="N49">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P49" t="str">
+        <f t="shared" si="7"/>
+        <v>Plymouth&amp;\bf{62}&amp;62.1&amp;735.1&amp;BS4&amp;73&amp;75\\</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B50">
         <v>83</v>
@@ -2789,7 +3043,7 @@
         <v>84</v>
       </c>
       <c r="F50" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G50">
@@ -2820,10 +3074,14 @@
       <c r="N50">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P50" t="str">
+        <f t="shared" si="7"/>
+        <v>Sheffield&amp;\bf{84}&amp;84.7&amp;1021.5&amp;BS4&amp;97&amp;98.9\\</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B51">
         <v>49</v>
@@ -2839,7 +3097,7 @@
         <v>50</v>
       </c>
       <c r="F51" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G51">
@@ -2870,10 +3128,14 @@
       <c r="N51">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P51" t="str">
+        <f t="shared" si="7"/>
+        <v>Southampton&amp;\bf{50}&amp;50.1&amp;315.9&amp;BS4&amp;60&amp;61.1\\</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="B52">
         <v>73</v>
@@ -2889,7 +3151,7 @@
         <v>73</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>best</v>
       </c>
       <c r="G52">
@@ -2920,10 +3182,14 @@
       <c r="N52">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P52" t="str">
+        <f t="shared" si="7"/>
+        <v>Sunderland&amp;\bf{73}&amp;73.7&amp;754.2&amp;BS4&amp;87&amp;89.1\\</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="B53">
         <v>68</v>
@@ -2939,7 +3205,7 @@
         <v>68</v>
       </c>
       <c r="F53" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>best</v>
       </c>
       <c r="G53">
@@ -2970,17 +3236,21 @@
       <c r="N53">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P53" t="str">
+        <f t="shared" si="7"/>
+        <v>York&amp;\bf{68}&amp;68&amp;755.1&amp;BS4&amp;77&amp;77.6\\</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="E54">
         <f>MIN('k2'!B23,'k2'!F23,'k2'!J23,'k2'!N23,'k2'!R23,'k2'!V23,'k2'!Z23,'k2'!AD23,'k2'!AH23,'k2'!AL23)</f>
         <v>169</v>
       </c>
       <c r="F54" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G54">
@@ -3011,17 +3281,21 @@
       <c r="N54">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P54" t="str">
+        <f t="shared" si="7"/>
+        <v>Belgrade&amp;\bf{169}&amp;172.3&amp;3614.1&amp;PG&amp;197&amp;197.5\\</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="E55">
         <f>MIN('k2'!B24,'k2'!F24,'k2'!J24,'k2'!N24,'k2'!R24,'k2'!V24,'k2'!Z24,'k2'!AD24,'k2'!AH24,'k2'!AL24)</f>
         <v>206</v>
       </c>
       <c r="F55" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G55">
@@ -3052,17 +3326,21 @@
       <c r="N55">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P55" t="str">
+        <f t="shared" si="7"/>
+        <v>Berlin&amp;\bf{206}&amp;207.1&amp;3611.6&amp;PG&amp;268&amp;270.4\\</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="E56">
         <f>MIN('k2'!B25,'k2'!F25,'k2'!J25,'k2'!N25,'k2'!R25,'k2'!V25,'k2'!Z25,'k2'!AD25,'k2'!AH25,'k2'!AL25)</f>
         <v>181</v>
       </c>
       <c r="F56" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G56">
@@ -3093,17 +3371,21 @@
       <c r="N56">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P56" t="str">
+        <f t="shared" si="7"/>
+        <v>Boston&amp;181&amp;194.6&amp;5707.7&amp;PG&amp;\bf{133}&amp;135\\</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E57">
         <f>MIN('k2'!B26,'k2'!F26,'k2'!J26,'k2'!N26,'k2'!R26,'k2'!V26,'k2'!Z26,'k2'!AD26,'k2'!AH26,'k2'!AL26)</f>
         <v>181</v>
       </c>
       <c r="F57" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G57">
@@ -3134,17 +3416,21 @@
       <c r="N57">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P57" t="str">
+        <f t="shared" si="7"/>
+        <v>Dublin&amp;181&amp;184.4&amp;5190.1&amp;PG&amp;\bf{166}&amp;166.8\\</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="E58">
         <f>MIN('k2'!B27,'k2'!F27,'k2'!J27,'k2'!N27,'k2'!R27,'k2'!V27,'k2'!Z27,'k2'!AD27,'k2'!AH27,'k2'!AL27)</f>
         <v>197</v>
       </c>
       <c r="F58" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G58">
@@ -3175,8 +3461,12 @@
       <c r="N58">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P58" t="str">
+        <f t="shared" si="7"/>
+        <v>Minsk&amp;\bf{197}&amp;201.1&amp;3602.4&amp;PG&amp;265&amp;266.4\\</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>24</v>
       </c>
@@ -3185,15 +3475,15 @@
         <v>70.45</v>
       </c>
       <c r="C59" s="1">
-        <f t="shared" ref="C59:J59" si="6">AVERAGE(C34:C58)</f>
+        <f t="shared" ref="C59:J59" si="8">AVERAGE(C34:C58)</f>
         <v>1</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.9030000000000005</v>
       </c>
       <c r="E59" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>94.2</v>
       </c>
       <c r="F59" s="1">
@@ -3201,36 +3491,39 @@
         <v>9</v>
       </c>
       <c r="G59" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>95.707999999999998</v>
       </c>
       <c r="H59" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.0976296404941266</v>
       </c>
       <c r="I59" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>704.00608000000011</v>
       </c>
       <c r="J59" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1680.9719999999998</v>
       </c>
       <c r="K59" s="1"/>
       <c r="L59" s="1">
-        <f t="shared" ref="L59" si="7">AVERAGE(L34:L58)</f>
+        <f t="shared" ref="L59" si="9">AVERAGE(L34:L58)</f>
         <v>109</v>
       </c>
       <c r="M59" s="1">
-        <f t="shared" ref="M59" si="8">AVERAGE(M34:M58)</f>
+        <f t="shared" ref="M59" si="10">AVERAGE(M34:M58)</f>
         <v>110.63600000000001</v>
       </c>
       <c r="N59" s="1">
-        <f t="shared" ref="N59" si="9">AVERAGE(N34:N58)</f>
+        <f t="shared" ref="N59" si="11">AVERAGE(N34:N58)</f>
         <v>1.0120000000000002</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -3242,7 +3535,7 @@
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2" t="s">
         <v>31</v>
@@ -3258,7 +3551,7 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>20</v>
       </c>
@@ -3301,10 +3594,13 @@
       <c r="N63" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P63" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B64">
         <v>138</v>
@@ -3351,10 +3647,14 @@
       <c r="N64">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P64" t="str">
+        <f>A64&amp;"&amp;"&amp;IF(E64&lt;=L64,"\bf{"&amp;E64&amp;"}",E64)&amp;"&amp;"&amp;ROUND(G64,1)&amp;"&amp;"&amp;ROUND(J64,1)&amp;"&amp;"&amp;K64&amp;"&amp;"&amp;IF(L64&lt;=E64,"\bf{"&amp;L64&amp;"}",L64)&amp;"&amp;"&amp;ROUND(M64,1)&amp;"\\"</f>
+        <v>Bath&amp;\bf{139}&amp;140.4&amp;434.8&amp;BS4&amp;159&amp;160\\</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="B65">
         <v>144</v>
@@ -3370,7 +3670,7 @@
         <v>147</v>
       </c>
       <c r="F65" t="str">
-        <f t="shared" ref="F65:F88" si="10">IF(E65=$B65,"best","")</f>
+        <f t="shared" ref="F65:F88" si="12">IF(E65=$B65,"best","")</f>
         <v/>
       </c>
       <c r="G65">
@@ -3401,10 +3701,14 @@
       <c r="N65">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P65" t="str">
+        <f t="shared" ref="P65:P88" si="13">A65&amp;"&amp;"&amp;IF(E65&lt;=L65,"\bf{"&amp;E65&amp;"}",E65)&amp;"&amp;"&amp;ROUND(G65,1)&amp;"&amp;"&amp;ROUND(J65,1)&amp;"&amp;"&amp;K65&amp;"&amp;"&amp;IF(L65&lt;=E65,"\bf{"&amp;L65&amp;"}",L65)&amp;"&amp;"&amp;ROUND(M65,1)&amp;"\\"</f>
+        <v>Belfast&amp;\bf{147}&amp;148.5&amp;2843.1&amp;BS4&amp;177&amp;179.6\\</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="B66">
         <v>76</v>
@@ -3420,7 +3724,7 @@
         <v>78</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G66">
@@ -3451,10 +3755,14 @@
       <c r="N66">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P66" t="str">
+        <f t="shared" si="13"/>
+        <v>Brighton&amp;\bf{78}&amp;79.3&amp;1393.7&amp;BS4&amp;92&amp;94.8\\</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="B67">
         <v>141</v>
@@ -3470,7 +3778,7 @@
         <v>145</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G67">
@@ -3501,10 +3809,14 @@
       <c r="N67">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P67" t="str">
+        <f t="shared" si="13"/>
+        <v>Bristol&amp;\bf{145}&amp;146.7&amp;979&amp;BS4&amp;175&amp;176.4\\</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B68">
         <v>155</v>
@@ -3520,7 +3832,7 @@
         <v>160</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G68">
@@ -3551,10 +3863,14 @@
       <c r="N68">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P68" t="str">
+        <f t="shared" si="13"/>
+        <v>Cardiff&amp;\bf{160}&amp;161.9&amp;1285&amp;BS4&amp;181&amp;183.2\\</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="B69">
         <v>145</v>
@@ -3570,7 +3886,7 @@
         <v>150</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G69">
@@ -3601,10 +3917,14 @@
       <c r="N69">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P69" t="str">
+        <f t="shared" si="13"/>
+        <v>Coventry&amp;\bf{150}&amp;150.6&amp;1394.3&amp;BS4&amp;170&amp;172.6\\</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B70">
         <v>154</v>
@@ -3620,7 +3940,7 @@
         <v>157</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G70">
@@ -3651,10 +3971,14 @@
       <c r="N70">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P70" t="str">
+        <f t="shared" si="13"/>
+        <v>Exeter&amp;\bf{157}&amp;158.3&amp;634&amp;BS4&amp;181&amp;182.3\\</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="B71">
         <v>170</v>
@@ -3670,7 +3994,7 @@
         <v>174</v>
       </c>
       <c r="F71" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G71">
@@ -3701,10 +4025,14 @@
       <c r="N71">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P71" t="str">
+        <f t="shared" si="13"/>
+        <v>Glasgow&amp;\bf{174}&amp;175.4&amp;550.8&amp;BS4&amp;197&amp;199.8\\</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B72">
         <v>149</v>
@@ -3720,7 +4048,7 @@
         <v>152</v>
       </c>
       <c r="F72" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G72">
@@ -3751,10 +4079,14 @@
       <c r="N72">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P72" t="str">
+        <f t="shared" si="13"/>
+        <v>Leeds&amp;\bf{152}&amp;152.4&amp;1737.2&amp;BS4&amp;186&amp;187.1\\</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B73">
         <v>145</v>
@@ -3770,7 +4102,7 @@
         <v>151</v>
       </c>
       <c r="F73" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G73">
@@ -3801,10 +4133,14 @@
       <c r="N73">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P73" t="str">
+        <f t="shared" si="13"/>
+        <v>Leicester&amp;\bf{151}&amp;152.6&amp;2846&amp;BS4&amp;175&amp;177.7\\</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="B74">
         <v>110</v>
@@ -3820,7 +4156,7 @@
         <v>112</v>
       </c>
       <c r="F74" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G74">
@@ -3851,10 +4187,14 @@
       <c r="N74">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P74" t="str">
+        <f t="shared" si="13"/>
+        <v>Liverpool&amp;\bf{112}&amp;114&amp;1673.1&amp;BS4&amp;132&amp;133\\</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="B75">
         <v>147</v>
@@ -3870,7 +4210,7 @@
         <v>154</v>
       </c>
       <c r="F75" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G75">
@@ -3901,10 +4241,14 @@
       <c r="N75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P75" t="str">
+        <f t="shared" si="13"/>
+        <v>Manchester&amp;\bf{154}&amp;156.4&amp;3302&amp;BS4&amp;177&amp;178.5\\</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="B76">
         <v>150</v>
@@ -3920,7 +4264,7 @@
         <v>153</v>
       </c>
       <c r="F76" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G76">
@@ -3951,10 +4295,14 @@
       <c r="N76">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P76" t="str">
+        <f t="shared" si="13"/>
+        <v>Newcastle&amp;\bf{153}&amp;154.8&amp;2103.6&amp;BS2&amp;169&amp;171.5\\</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B77">
         <v>160</v>
@@ -3970,7 +4318,7 @@
         <v>165</v>
       </c>
       <c r="F77" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G77">
@@ -4001,10 +4349,14 @@
       <c r="N77">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P77" t="str">
+        <f t="shared" si="13"/>
+        <v>Nottingham&amp;\bf{165}&amp;166.6&amp;2718.3&amp;BS4&amp;193&amp;195.2\\</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="B78">
         <v>89</v>
@@ -4020,7 +4372,7 @@
         <v>89</v>
       </c>
       <c r="F78" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>best</v>
       </c>
       <c r="G78">
@@ -4051,10 +4403,14 @@
       <c r="N78">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P78" t="str">
+        <f t="shared" si="13"/>
+        <v>Oxford&amp;\bf{89}&amp;89.2&amp;114.9&amp;BS2&amp;99&amp;100.8\\</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B79">
         <v>115</v>
@@ -4101,10 +4457,14 @@
       <c r="N79">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P79" t="str">
+        <f t="shared" si="13"/>
+        <v>Plymouth&amp;\bf{115}&amp;116&amp;1725.7&amp;BS4&amp;135&amp;137\\</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B80">
         <v>156</v>
@@ -4120,7 +4480,7 @@
         <v>160</v>
       </c>
       <c r="F80" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G80">
@@ -4151,10 +4511,14 @@
       <c r="N80">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P80" t="str">
+        <f t="shared" si="13"/>
+        <v>Sheffield&amp;\bf{160}&amp;161.6&amp;1351.2&amp;BS4&amp;180&amp;182.2\\</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B81">
         <v>96</v>
@@ -4170,7 +4534,7 @@
         <v>97</v>
       </c>
       <c r="F81" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G81">
@@ -4201,10 +4565,14 @@
       <c r="N81">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P81" t="str">
+        <f t="shared" si="13"/>
+        <v>Southampton&amp;\bf{97}&amp;97.8&amp;653.1&amp;BS4&amp;112&amp;113.2\\</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="B82">
         <v>138</v>
@@ -4220,7 +4588,7 @@
         <v>142</v>
       </c>
       <c r="F82" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G82">
@@ -4251,10 +4619,14 @@
       <c r="N82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P82" t="str">
+        <f t="shared" si="13"/>
+        <v>Sunderland&amp;\bf{142}&amp;142.5&amp;3539.1&amp;BS4&amp;162&amp;163.6\\</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="B83">
         <v>129</v>
@@ -4270,7 +4642,7 @@
         <v>129</v>
       </c>
       <c r="F83" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>best</v>
       </c>
       <c r="G83">
@@ -4301,17 +4673,21 @@
       <c r="N83">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P83" t="str">
+        <f t="shared" si="13"/>
+        <v>York&amp;\bf{129}&amp;130.1&amp;630.5&amp;BS4&amp;144&amp;145.8\\</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="E84">
         <f>MIN('k4'!B23,'k4'!F23,'k4'!J23,'k4'!N23,'k4'!R23,'k4'!V23,'k4'!Z23,'k4'!AD23,'k4'!AH23,'k4'!AL23)</f>
         <v>344</v>
       </c>
       <c r="F84" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G84">
@@ -4342,17 +4718,21 @@
       <c r="N84">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P84" t="str">
+        <f t="shared" si="13"/>
+        <v>Belgrade&amp;\bf{344}&amp;346.3&amp;3610.9&amp;SG&amp;397&amp;400.1\\</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="E85">
         <f>MIN('k4'!B24,'k4'!F24,'k4'!J24,'k4'!N24,'k4'!R24,'k4'!V24,'k4'!Z24,'k4'!AD24,'k4'!AH24,'k4'!AL24)</f>
         <v>408</v>
       </c>
       <c r="F85" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G85">
@@ -4383,17 +4763,21 @@
       <c r="N85">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P85" t="str">
+        <f t="shared" si="13"/>
+        <v>Berlin&amp;\bf{408}&amp;409.2&amp;3612&amp;PG&amp;501&amp;503.4\\</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="E86">
         <f>MIN('k4'!B25,'k4'!F25,'k4'!J25,'k4'!N25,'k4'!R25,'k4'!V25,'k4'!Z25,'k4'!AD25,'k4'!AH25,'k4'!AL25)</f>
         <v>341</v>
       </c>
       <c r="F86" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G86">
@@ -4424,17 +4808,21 @@
       <c r="N86">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P86" t="str">
+        <f t="shared" si="13"/>
+        <v>Boston&amp;341&amp;341&amp;9340&amp;PG&amp;\bf{255}&amp;255.4\\</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E87">
         <f>MIN('k4'!B26,'k4'!F26,'k4'!J26,'k4'!N26,'k4'!R26,'k4'!V26,'k4'!Z26,'k4'!AD26,'k4'!AH26,'k4'!AL26)</f>
         <v>363</v>
       </c>
       <c r="F87" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G87">
@@ -4465,17 +4853,21 @@
       <c r="N87">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P87" t="str">
+        <f t="shared" si="13"/>
+        <v>Dublin&amp;363&amp;363&amp;10035.5&amp;PG&amp;\bf{317}&amp;318.5\\</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="E88">
         <f>MIN('k4'!B27,'k4'!F27,'k4'!J27,'k4'!N27,'k4'!R27,'k4'!V27,'k4'!Z27,'k4'!AD27,'k4'!AH27,'k4'!AL27)</f>
         <v>387</v>
       </c>
       <c r="F88" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G88">
@@ -4506,8 +4898,12 @@
       <c r="N88">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P88" t="str">
+        <f t="shared" si="13"/>
+        <v>Minsk&amp;\bf{387}&amp;391.5&amp;3601.6&amp;PG&amp;506&amp;509.4\\</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>24</v>
       </c>
@@ -4516,15 +4912,15 @@
         <v>135.35</v>
       </c>
       <c r="C89" s="1">
-        <f t="shared" ref="C89" si="11">AVERAGE(C64:C88)</f>
+        <f t="shared" ref="C89" si="14">AVERAGE(C64:C88)</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="D89" s="1">
-        <f t="shared" ref="D89" si="12">AVERAGE(D64:D88)</f>
+        <f t="shared" ref="D89" si="15">AVERAGE(D64:D88)</f>
         <v>1894.1545000000006</v>
       </c>
       <c r="E89" s="1">
-        <f t="shared" ref="E89" si="13">AVERAGE(E64:E88)</f>
+        <f t="shared" ref="E89" si="16">AVERAGE(E64:E88)</f>
         <v>184.48</v>
       </c>
       <c r="F89" s="1">
@@ -4532,33 +4928,36 @@
         <v>3</v>
       </c>
       <c r="G89" s="1">
-        <f t="shared" ref="G89" si="14">AVERAGE(G64:G88)</f>
+        <f t="shared" ref="G89" si="17">AVERAGE(G64:G88)</f>
         <v>185.84400000000002</v>
       </c>
       <c r="H89" s="1">
-        <f t="shared" ref="H89" si="15">AVERAGE(H64:H88)</f>
+        <f t="shared" ref="H89" si="18">AVERAGE(H64:H88)</f>
         <v>0.8650831775144211</v>
       </c>
       <c r="I89" s="1">
-        <f t="shared" ref="I89" si="16">AVERAGE(I64:I88)</f>
+        <f t="shared" ref="I89" si="19">AVERAGE(I64:I88)</f>
         <v>1158.3819599999999</v>
       </c>
       <c r="J89" s="1">
-        <f t="shared" ref="J89" si="17">AVERAGE(J64:J88)</f>
+        <f t="shared" ref="J89" si="20">AVERAGE(J64:J88)</f>
         <v>2484.37428</v>
       </c>
       <c r="K89" s="1"/>
       <c r="L89" s="1">
-        <f t="shared" ref="L89" si="18">AVERAGE(L64:L88)</f>
+        <f t="shared" ref="L89" si="21">AVERAGE(L64:L88)</f>
         <v>206.88</v>
       </c>
       <c r="M89" s="1">
-        <f t="shared" ref="M89" si="19">AVERAGE(M64:M88)</f>
+        <f t="shared" ref="M89" si="22">AVERAGE(M64:M88)</f>
         <v>208.84399999999994</v>
       </c>
       <c r="N89" s="1">
-        <f t="shared" ref="N89" si="20">AVERAGE(N64:N88)</f>
+        <f t="shared" ref="N89" si="23">AVERAGE(N64:N88)</f>
         <v>1.2959999999999996</v>
+      </c>
+      <c r="P89" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new results and comment on paper
</commit_message>
<xml_diff>
--- a/algorithms/results/comparison.xlsx
+++ b/algorithms/results/comparison.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\akcijanje\nauka\moji radovi\aktivno\k-domination\algorithms\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\radovi\K-domination\k-domination\algorithms\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E402D7-8BF2-4265-BDD9-F03DCD7FE6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3555" windowWidth="29040" windowHeight="15840" xr2:uid="{9811A06C-B274-406A-BE4D-18F0FA4A89B1}"/>
+    <workbookView xWindow="-28920" yWindow="-3555" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="k2" sheetId="3" r:id="rId4"/>
     <sheet name="k4" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -297,7 +296,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -315,12 +314,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -335,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -344,9 +349,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalan" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -657,11 +664,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C114BA-E20E-4760-908C-9E2FAA6D010C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:XFD78"/>
+    <sheetView tabSelected="1" topLeftCell="E63" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M74" sqref="M74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1858,17 +1865,17 @@
         <v>48</v>
       </c>
       <c r="L24">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="M24">
-        <v>100.3</v>
+        <v>103.4</v>
       </c>
       <c r="N24">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="P24" t="str">
         <f t="shared" si="1"/>
-        <v>Belgrade&amp;\bf{85}&amp;88.4&amp;PG&amp;99&amp;100.3\\</v>
+        <v>Belgrade&amp;\bf{85}&amp;88.4&amp;PG&amp;103&amp;103.4\\</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -1900,20 +1907,20 @@
         <v>3609.4533333333334</v>
       </c>
       <c r="K25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L25">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="M25">
-        <v>147</v>
+        <v>125.9</v>
       </c>
       <c r="N25">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="P25" t="str">
         <f t="shared" si="1"/>
-        <v>Berlin&amp;\bf{102}&amp;104.5&amp;SG&amp;146&amp;147\\</v>
+        <v>Berlin&amp;\bf{102}&amp;104.5&amp;PG&amp;125&amp;125.9\\</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -1945,20 +1952,20 @@
         <v>3685.5722222222216</v>
       </c>
       <c r="K26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L26">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="M26">
-        <v>72.599999999999994</v>
+        <v>102.7</v>
       </c>
       <c r="N26">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" si="1"/>
-        <v>Boston&amp;99&amp;101.2&amp;SG&amp;\bf{71}&amp;72.6\\</v>
+        <v>Boston&amp;\bf{99}&amp;101.2&amp;PG&amp;101&amp;102.7\\</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -1993,17 +2000,17 @@
         <v>48</v>
       </c>
       <c r="L27">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="M27">
-        <v>90.2</v>
+        <v>113.8</v>
       </c>
       <c r="N27">
-        <v>1.8</v>
+        <v>1.2</v>
       </c>
       <c r="P27" t="str">
         <f t="shared" si="1"/>
-        <v>Dublin&amp;93&amp;99&amp;PG&amp;\bf{88}&amp;90.2\\</v>
+        <v>Dublin&amp;\bf{93}&amp;99&amp;PG&amp;112&amp;113.8\\</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -2035,20 +2042,21 @@
         <v>3602.3222222222225</v>
       </c>
       <c r="K28" t="s">
-        <v>49</v>
-      </c>
-      <c r="L28">
+        <v>48</v>
+      </c>
+      <c r="L28" s="4">
         <v>138</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="4">
         <v>139.30000000000001</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="4">
         <v>1.1000000000000001</v>
       </c>
+      <c r="O28" s="5"/>
       <c r="P28" t="str">
         <f t="shared" si="1"/>
-        <v>Minsk&amp;\bf{100}&amp;102&amp;SG&amp;138&amp;139.3\\</v>
+        <v>Minsk&amp;\bf{100}&amp;102&amp;PG&amp;138&amp;139.3\\</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -2094,15 +2102,15 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1">
         <f t="shared" si="3"/>
-        <v>126.68</v>
+        <v>128.16</v>
       </c>
       <c r="M29" s="1">
         <f t="shared" ref="M29" si="4">AVERAGE(M4:M28)</f>
-        <v>128.428</v>
+        <v>129.85599999999999</v>
       </c>
       <c r="N29" s="1">
         <f t="shared" ref="N29" si="5">AVERAGE(N4:N28)</f>
-        <v>1.1239999999999997</v>
+        <v>1.0719999999999998</v>
       </c>
       <c r="P29" t="s">
         <v>75</v>
@@ -3295,17 +3303,17 @@
         <v>48</v>
       </c>
       <c r="L54">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M54">
-        <v>197.5</v>
+        <v>197.3</v>
       </c>
       <c r="N54">
         <v>0.9</v>
       </c>
       <c r="P54" t="str">
         <f t="shared" si="7"/>
-        <v>Belgrade&amp;\bf{169}&amp;172.3&amp;PG&amp;197&amp;197.5\\</v>
+        <v>Belgrade&amp;\bf{169}&amp;172.3&amp;PG&amp;196&amp;197.3\\</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -3340,17 +3348,17 @@
         <v>48</v>
       </c>
       <c r="L55">
-        <v>268</v>
+        <v>239</v>
       </c>
       <c r="M55">
-        <v>270.39999999999998</v>
+        <v>240.1</v>
       </c>
       <c r="N55">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="P55" t="str">
         <f t="shared" si="7"/>
-        <v>Berlin&amp;\bf{206}&amp;207.1&amp;PG&amp;268&amp;270.4\\</v>
+        <v>Berlin&amp;\bf{206}&amp;207.1&amp;PG&amp;239&amp;240.1\\</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -3385,17 +3393,17 @@
         <v>48</v>
       </c>
       <c r="L56">
-        <v>133</v>
+        <v>190</v>
       </c>
       <c r="M56">
-        <v>135</v>
+        <v>191.6</v>
       </c>
       <c r="N56">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="P56" t="str">
         <f t="shared" si="7"/>
-        <v>Boston&amp;181&amp;194.6&amp;PG&amp;\bf{133}&amp;135\\</v>
+        <v>Boston&amp;\bf{181}&amp;194.6&amp;PG&amp;190&amp;191.6\\</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -3430,17 +3438,17 @@
         <v>48</v>
       </c>
       <c r="L57">
-        <v>166</v>
+        <v>209</v>
       </c>
       <c r="M57">
-        <v>166.8</v>
+        <v>211.3</v>
       </c>
       <c r="N57">
-        <v>0.4</v>
+        <v>2.7</v>
       </c>
       <c r="P57" t="str">
         <f t="shared" si="7"/>
-        <v>Dublin&amp;181&amp;184.4&amp;PG&amp;\bf{166}&amp;166.8\\</v>
+        <v>Dublin&amp;\bf{181}&amp;184.4&amp;PG&amp;209&amp;211.3\\</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -3474,13 +3482,13 @@
       <c r="K58" t="s">
         <v>48</v>
       </c>
-      <c r="L58">
+      <c r="L58" s="4">
         <v>265</v>
       </c>
-      <c r="M58">
+      <c r="M58" s="4">
         <v>266.39999999999998</v>
       </c>
-      <c r="N58">
+      <c r="N58" s="4">
         <v>1.3</v>
       </c>
       <c r="P58" t="str">
@@ -3531,15 +3539,15 @@
       <c r="K59" s="1"/>
       <c r="L59" s="1">
         <f t="shared" ref="L59" si="9">AVERAGE(L34:L58)</f>
-        <v>109</v>
+        <v>111.8</v>
       </c>
       <c r="M59" s="1">
         <f t="shared" ref="M59" si="10">AVERAGE(M34:M58)</f>
-        <v>110.63600000000001</v>
+        <v>113.46</v>
       </c>
       <c r="N59" s="1">
         <f t="shared" ref="N59" si="11">AVERAGE(N34:N58)</f>
-        <v>1.0120000000000002</v>
+        <v>1.0880000000000001</v>
       </c>
       <c r="P59" t="s">
         <v>75</v>
@@ -4732,17 +4740,17 @@
         <v>49</v>
       </c>
       <c r="L84">
-        <v>397</v>
+        <v>372</v>
       </c>
       <c r="M84">
-        <v>400.1</v>
+        <v>374.5</v>
       </c>
       <c r="N84">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="P84" t="str">
         <f t="shared" si="13"/>
-        <v>Belgrade&amp;\bf{344}&amp;346.3&amp;SG&amp;397&amp;400.1\\</v>
+        <v>Belgrade&amp;\bf{344}&amp;346.3&amp;SG&amp;372&amp;374.5\\</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
@@ -4777,17 +4785,17 @@
         <v>48</v>
       </c>
       <c r="L85">
-        <v>501</v>
+        <v>444</v>
       </c>
       <c r="M85">
-        <v>503.4</v>
+        <v>446.2</v>
       </c>
       <c r="N85">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="P85" t="str">
         <f t="shared" si="13"/>
-        <v>Berlin&amp;\bf{408}&amp;409.2&amp;PG&amp;501&amp;503.4\\</v>
+        <v>Berlin&amp;\bf{408}&amp;409.2&amp;PG&amp;444&amp;446.2\\</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
@@ -4822,17 +4830,17 @@
         <v>48</v>
       </c>
       <c r="L86">
-        <v>255</v>
+        <v>367</v>
       </c>
       <c r="M86">
-        <v>255.4</v>
+        <v>368.7</v>
       </c>
       <c r="N86">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="P86" t="str">
         <f t="shared" si="13"/>
-        <v>Boston&amp;341&amp;341&amp;PG&amp;\bf{255}&amp;255.4\\</v>
+        <v>Boston&amp;\bf{341}&amp;341&amp;PG&amp;367&amp;368.7\\</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
@@ -4866,13 +4874,13 @@
       <c r="K87" t="s">
         <v>48</v>
       </c>
-      <c r="L87">
+      <c r="L87" s="4">
         <v>317</v>
       </c>
-      <c r="M87">
+      <c r="M87" s="4">
         <v>318.5</v>
       </c>
-      <c r="N87">
+      <c r="N87" s="4">
         <v>1.5</v>
       </c>
       <c r="P87" t="str">
@@ -4911,13 +4919,13 @@
       <c r="K88" t="s">
         <v>48</v>
       </c>
-      <c r="L88">
+      <c r="L88" s="4">
         <v>506</v>
       </c>
-      <c r="M88">
+      <c r="M88" s="4">
         <v>509.4</v>
       </c>
-      <c r="N88">
+      <c r="N88" s="4">
         <v>2.9</v>
       </c>
       <c r="P88" t="str">
@@ -4968,34 +4976,34 @@
       <c r="K89" s="1"/>
       <c r="L89" s="1">
         <f t="shared" ref="L89" si="21">AVERAGE(L64:L88)</f>
-        <v>206.88</v>
+        <v>208.08</v>
       </c>
       <c r="M89" s="1">
         <f t="shared" ref="M89" si="22">AVERAGE(M64:M88)</f>
-        <v>208.84399999999994</v>
+        <v>210.06399999999996</v>
       </c>
       <c r="N89" s="1">
         <f t="shared" ref="N89" si="23">AVERAGE(N64:N88)</f>
-        <v>1.2959999999999996</v>
+        <v>1.3359999999999996</v>
       </c>
       <c r="P89" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L1:O89">
+  <sortState ref="L1:O89">
     <sortCondition ref="L1:L89"/>
   </sortState>
   <mergeCells count="9">
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="B32:D32"/>
     <mergeCell ref="B61:J61"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="E32:J32"/>
     <mergeCell ref="E62:J62"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B31:J31"/>
-    <mergeCell ref="E2:J2"/>
-    <mergeCell ref="B32:D32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5003,7 +5011,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7833E92D-83B8-4848-83C5-FC9D01B5B689}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5061,7 +5069,7 @@
         <v>10035.541000000001</v>
       </c>
       <c r="G2">
-        <f>SUM(D2:F2)</f>
+        <f t="shared" ref="G2:G26" si="0">SUM(D2:F2)</f>
         <v>18527.432000000001</v>
       </c>
     </row>
@@ -5088,7 +5096,7 @@
         <v>9339.9700000000012</v>
       </c>
       <c r="G3">
-        <f>SUM(D3:F3)</f>
+        <f t="shared" si="0"/>
         <v>18360.849999999999</v>
       </c>
     </row>
@@ -5115,7 +5123,7 @@
         <v>3574.4879999999998</v>
       </c>
       <c r="G4">
-        <f>SUM(D4:F4)</f>
+        <f t="shared" si="0"/>
         <v>9881.607</v>
       </c>
     </row>
@@ -5142,7 +5150,7 @@
         <v>3441.4929999999995</v>
       </c>
       <c r="G5">
-        <f>SUM(D5:F5)</f>
+        <f t="shared" si="0"/>
         <v>9499.7439999999988</v>
       </c>
     </row>
@@ -5169,7 +5177,7 @@
         <v>3364.1230000000005</v>
       </c>
       <c r="G6">
-        <f>SUM(D6:F6)</f>
+        <f t="shared" si="0"/>
         <v>8315.0580000000009</v>
       </c>
     </row>
@@ -5196,7 +5204,7 @@
         <v>2584.7870000000007</v>
       </c>
       <c r="G7">
-        <f>SUM(D7:F7)</f>
+        <f t="shared" si="0"/>
         <v>5037.5600000000004</v>
       </c>
     </row>
@@ -5223,7 +5231,7 @@
         <v>1827.64</v>
       </c>
       <c r="G8">
-        <f>SUM(D8:F8)</f>
+        <f t="shared" si="0"/>
         <v>3038.076</v>
       </c>
     </row>
@@ -5250,7 +5258,7 @@
         <v>1800.3589999999999</v>
       </c>
       <c r="G9">
-        <f>SUM(D9:F9)</f>
+        <f t="shared" si="0"/>
         <v>2732.4830000000002</v>
       </c>
     </row>
@@ -5277,7 +5285,7 @@
         <v>2464.1019999999999</v>
       </c>
       <c r="G10">
-        <f>SUM(D10:F10)</f>
+        <f t="shared" si="0"/>
         <v>2695.9579999999996</v>
       </c>
     </row>
@@ -5304,7 +5312,7 @@
         <v>1729.2720000000002</v>
       </c>
       <c r="G11">
-        <f>SUM(D11:F11)</f>
+        <f t="shared" si="0"/>
         <v>2424.71</v>
       </c>
     </row>
@@ -5331,7 +5339,7 @@
         <v>1147.6460000000002</v>
       </c>
       <c r="G12">
-        <f>SUM(D12:F12)</f>
+        <f t="shared" si="0"/>
         <v>1614.8010000000002</v>
       </c>
     </row>
@@ -5358,7 +5366,7 @@
         <v>1078.0520000000001</v>
       </c>
       <c r="G13">
-        <f>SUM(D13:F13)</f>
+        <f t="shared" si="0"/>
         <v>1502.145</v>
       </c>
     </row>
@@ -5385,7 +5393,7 @@
         <v>981.00600000000009</v>
       </c>
       <c r="G14">
-        <f>SUM(D14:F14)</f>
+        <f t="shared" si="0"/>
         <v>1413.259</v>
       </c>
     </row>
@@ -5412,7 +5420,7 @@
         <v>638.25</v>
       </c>
       <c r="G15">
-        <f>SUM(D15:F15)</f>
+        <f t="shared" si="0"/>
         <v>1339.1009999999999</v>
       </c>
     </row>
@@ -5439,7 +5447,7 @@
         <v>826.95299999999986</v>
       </c>
       <c r="G16">
-        <f>SUM(D16:F16)</f>
+        <f t="shared" si="0"/>
         <v>1271.9449999999999</v>
       </c>
     </row>
@@ -5466,7 +5474,7 @@
         <v>858.97299999999996</v>
       </c>
       <c r="G17">
-        <f>SUM(D17:F17)</f>
+        <f t="shared" si="0"/>
         <v>1240.1619999999998</v>
       </c>
     </row>
@@ -5493,7 +5501,7 @@
         <v>850.46400000000017</v>
       </c>
       <c r="G18">
-        <f>SUM(D18:F18)</f>
+        <f t="shared" si="0"/>
         <v>1217.7160000000001</v>
       </c>
     </row>
@@ -5520,7 +5528,7 @@
         <v>919.92699999999991</v>
       </c>
       <c r="G19">
-        <f>SUM(D19:F19)</f>
+        <f t="shared" si="0"/>
         <v>1180.1949999999999</v>
       </c>
     </row>
@@ -5547,7 +5555,7 @@
         <v>679.32499999999993</v>
       </c>
       <c r="G20">
-        <f>SUM(D20:F20)</f>
+        <f t="shared" si="0"/>
         <v>903.16899999999987</v>
       </c>
     </row>
@@ -5574,7 +5582,7 @@
         <v>387.58800000000008</v>
       </c>
       <c r="G21">
-        <f>SUM(D21:F21)</f>
+        <f t="shared" si="0"/>
         <v>725.13700000000006</v>
       </c>
     </row>
@@ -5601,7 +5609,7 @@
         <v>285.74400000000003</v>
       </c>
       <c r="G22">
-        <f>SUM(D22:F22)</f>
+        <f t="shared" si="0"/>
         <v>603.36400000000003</v>
       </c>
     </row>
@@ -5628,7 +5636,7 @@
         <v>376.05700000000002</v>
       </c>
       <c r="G23">
-        <f>SUM(D23:F23)</f>
+        <f t="shared" si="0"/>
         <v>577.053</v>
       </c>
     </row>
@@ -5655,7 +5663,7 @@
         <v>359.89000000000004</v>
       </c>
       <c r="G24">
-        <f>SUM(D24:F24)</f>
+        <f t="shared" si="0"/>
         <v>500.21400000000006</v>
       </c>
     </row>
@@ -5682,7 +5690,7 @@
         <v>203.32399999999998</v>
       </c>
       <c r="G25">
-        <f>SUM(D25:F25)</f>
+        <f t="shared" si="0"/>
         <v>358.88299999999998</v>
       </c>
     </row>
@@ -5709,12 +5717,12 @@
         <v>23.79</v>
       </c>
       <c r="G26">
-        <f>SUM(D26:F26)</f>
+        <f t="shared" si="0"/>
         <v>49.478000000000002</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:G26">
+  <sortState ref="C2:G26">
     <sortCondition descending="1" ref="G1:G26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5722,7 +5730,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E0A399-1392-421F-BE16-4A68D42F8610}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO27"/>
   <sheetViews>
     <sheetView topLeftCell="L1" workbookViewId="0">
@@ -9065,7 +9073,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1899936-B5F7-44DD-83C8-1FC6D40F114A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12404,7 +12412,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E005DE69-62B8-4E9D-ACDF-70327098D6E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO27"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
added results for Minsk and Dublin
</commit_message>
<xml_diff>
--- a/algorithms/results/comparison.xlsx
+++ b/algorithms/results/comparison.xlsx
@@ -317,18 +317,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -352,21 +346,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalan" xfId="0" builtinId="0"/>
@@ -683,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P78" sqref="P78"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,31 +689,31 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -812,7 +805,7 @@
       <c r="L4">
         <v>43</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="4">
         <v>44.6</v>
       </c>
       <c r="N4">
@@ -866,7 +859,7 @@
       <c r="L5">
         <v>48</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="4">
         <v>50.2</v>
       </c>
       <c r="N5">
@@ -920,7 +913,7 @@
       <c r="L6">
         <v>28</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="4">
         <v>28.2</v>
       </c>
       <c r="N6">
@@ -974,7 +967,7 @@
       <c r="L7">
         <v>46</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="4">
         <v>47.4</v>
       </c>
       <c r="N7">
@@ -1028,7 +1021,7 @@
       <c r="L8">
         <v>48</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="4">
         <v>50.6</v>
       </c>
       <c r="N8">
@@ -1082,7 +1075,7 @@
       <c r="L9">
         <v>44</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="4">
         <v>44.8</v>
       </c>
       <c r="N9">
@@ -1136,7 +1129,7 @@
       <c r="L10">
         <v>50</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="4">
         <v>50.6</v>
       </c>
       <c r="N10">
@@ -1190,7 +1183,7 @@
       <c r="L11">
         <v>58</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="4">
         <v>59.2</v>
       </c>
       <c r="N11">
@@ -1244,7 +1237,7 @@
       <c r="L12">
         <v>51</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="4">
         <v>52.4</v>
       </c>
       <c r="N12">
@@ -1298,7 +1291,7 @@
       <c r="L13">
         <v>51</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="4">
         <v>51.5</v>
       </c>
       <c r="N13">
@@ -1352,7 +1345,7 @@
       <c r="L14">
         <v>38</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="4">
         <v>38.4</v>
       </c>
       <c r="N14">
@@ -1406,7 +1399,7 @@
       <c r="L15">
         <v>45</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="4">
         <v>45.9</v>
       </c>
       <c r="N15">
@@ -1460,7 +1453,7 @@
       <c r="L16">
         <v>51</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M16" s="4">
         <v>52.6</v>
       </c>
       <c r="N16">
@@ -1514,7 +1507,7 @@
       <c r="L17">
         <v>55</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M17" s="4">
         <v>56.6</v>
       </c>
       <c r="N17">
@@ -1568,7 +1561,7 @@
       <c r="L18">
         <v>27</v>
       </c>
-      <c r="M18" s="7">
+      <c r="M18" s="4">
         <v>27.9</v>
       </c>
       <c r="N18">
@@ -1622,7 +1615,7 @@
       <c r="L19">
         <v>39</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="4">
         <v>40.299999999999997</v>
       </c>
       <c r="N19">
@@ -1676,7 +1669,7 @@
       <c r="L20">
         <v>51</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M20" s="4">
         <v>52.5</v>
       </c>
       <c r="N20">
@@ -1730,7 +1723,7 @@
       <c r="L21">
         <v>28</v>
       </c>
-      <c r="M21" s="7">
+      <c r="M21" s="4">
         <v>29.6</v>
       </c>
       <c r="N21">
@@ -1784,7 +1777,7 @@
       <c r="L22">
         <v>46</v>
       </c>
-      <c r="M22" s="7">
+      <c r="M22" s="4">
         <v>46.3</v>
       </c>
       <c r="N22">
@@ -1838,7 +1831,7 @@
       <c r="L23">
         <v>39</v>
       </c>
-      <c r="M23" s="7">
+      <c r="M23" s="4">
         <v>39.1</v>
       </c>
       <c r="N23">
@@ -2061,18 +2054,18 @@
         <v>48</v>
       </c>
       <c r="L28" s="2">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="M28" s="2">
-        <v>139.30000000000001</v>
+        <v>126</v>
       </c>
       <c r="N28" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="O28" s="3"/>
+        <v>0.9</v>
+      </c>
+      <c r="O28" s="2"/>
       <c r="P28" t="str">
         <f t="shared" si="1"/>
-        <v>Minsk&amp;\bf{100}&amp;102&amp;PG&amp;138&amp;139.3\\</v>
+        <v>Minsk&amp;\bf{100}&amp;102&amp;PG&amp;125&amp;126\\</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -2118,15 +2111,15 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1">
         <f t="shared" si="3"/>
-        <v>58.6</v>
+        <v>58.08</v>
       </c>
       <c r="M29" s="1">
         <f t="shared" ref="M29" si="4">AVERAGE(M4:M28)</f>
-        <v>59.751999999999995</v>
+        <v>59.22</v>
       </c>
       <c r="N29" s="1">
         <f t="shared" ref="N29" si="5">AVERAGE(N4:N28)</f>
-        <v>0.75600000000000012</v>
+        <v>0.748</v>
       </c>
       <c r="P29" t="s">
         <v>75</v>
@@ -2134,31 +2127,31 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4" t="s">
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -2304,7 +2297,7 @@
       <c r="L35">
         <v>96</v>
       </c>
-      <c r="M35" s="6">
+      <c r="M35" s="3">
         <v>97.6</v>
       </c>
       <c r="N35">
@@ -2358,7 +2351,7 @@
       <c r="L36">
         <v>49</v>
       </c>
-      <c r="M36" s="6">
+      <c r="M36" s="3">
         <v>49.4</v>
       </c>
       <c r="N36">
@@ -2412,7 +2405,7 @@
       <c r="L37">
         <v>91</v>
       </c>
-      <c r="M37" s="6">
+      <c r="M37" s="3">
         <v>94</v>
       </c>
       <c r="N37">
@@ -2466,7 +2459,7 @@
       <c r="L38">
         <v>92</v>
       </c>
-      <c r="M38" s="6">
+      <c r="M38" s="3">
         <v>95.6</v>
       </c>
       <c r="N38">
@@ -2520,7 +2513,7 @@
       <c r="L39">
         <v>84</v>
       </c>
-      <c r="M39" s="8">
+      <c r="M39" s="5">
         <v>85.1</v>
       </c>
       <c r="N39">
@@ -2574,7 +2567,7 @@
       <c r="L40">
         <v>94</v>
       </c>
-      <c r="M40" s="8">
+      <c r="M40" s="5">
         <v>95.7</v>
       </c>
       <c r="N40">
@@ -2628,7 +2621,7 @@
       <c r="L41">
         <v>108</v>
       </c>
-      <c r="M41" s="8">
+      <c r="M41" s="5">
         <v>110.6</v>
       </c>
       <c r="N41">
@@ -2682,7 +2675,7 @@
       <c r="L42">
         <v>98</v>
       </c>
-      <c r="M42" s="6">
+      <c r="M42" s="3">
         <v>99.6</v>
       </c>
       <c r="N42">
@@ -2736,7 +2729,7 @@
       <c r="L43">
         <v>93</v>
       </c>
-      <c r="M43" s="9">
+      <c r="M43" s="6">
         <v>94.1</v>
       </c>
       <c r="N43">
@@ -2790,7 +2783,7 @@
       <c r="L44">
         <v>71</v>
       </c>
-      <c r="M44" s="9">
+      <c r="M44" s="6">
         <v>72</v>
       </c>
       <c r="N44">
@@ -2844,7 +2837,7 @@
       <c r="L45">
         <v>90</v>
       </c>
-      <c r="M45" s="9">
+      <c r="M45" s="6">
         <v>91.5</v>
       </c>
       <c r="N45">
@@ -2898,7 +2891,7 @@
       <c r="L46">
         <v>94</v>
       </c>
-      <c r="M46" s="9">
+      <c r="M46" s="6">
         <v>95.4</v>
       </c>
       <c r="N46">
@@ -2952,7 +2945,7 @@
       <c r="L47">
         <v>102</v>
       </c>
-      <c r="M47" s="9">
+      <c r="M47" s="6">
         <v>103.3</v>
       </c>
       <c r="N47">
@@ -3006,7 +2999,7 @@
       <c r="L48">
         <v>54</v>
       </c>
-      <c r="M48" s="9">
+      <c r="M48" s="6">
         <v>54.9</v>
       </c>
       <c r="N48">
@@ -3060,7 +3053,7 @@
       <c r="L49">
         <v>73</v>
       </c>
-      <c r="M49" s="9">
+      <c r="M49" s="6">
         <v>75</v>
       </c>
       <c r="N49">
@@ -3114,7 +3107,7 @@
       <c r="L50">
         <v>97</v>
       </c>
-      <c r="M50" s="9">
+      <c r="M50" s="6">
         <v>98.9</v>
       </c>
       <c r="N50">
@@ -3168,7 +3161,7 @@
       <c r="L51">
         <v>60</v>
       </c>
-      <c r="M51" s="9">
+      <c r="M51" s="6">
         <v>61.1</v>
       </c>
       <c r="N51">
@@ -3222,7 +3215,7 @@
       <c r="L52">
         <v>87</v>
       </c>
-      <c r="M52" s="9">
+      <c r="M52" s="6">
         <v>89.1</v>
       </c>
       <c r="N52">
@@ -3276,7 +3269,7 @@
       <c r="L53">
         <v>77</v>
       </c>
-      <c r="M53" s="9">
+      <c r="M53" s="6">
         <v>77.599999999999994</v>
       </c>
       <c r="N53">
@@ -3499,17 +3492,17 @@
         <v>48</v>
       </c>
       <c r="L58" s="2">
-        <v>265</v>
+        <v>238</v>
       </c>
       <c r="M58" s="2">
-        <v>266.39999999999998</v>
+        <v>240.4</v>
       </c>
       <c r="N58" s="2">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="P58" t="str">
         <f t="shared" si="7"/>
-        <v>Minsk&amp;\bf{197}&amp;201.1&amp;PG&amp;265&amp;266.4\\</v>
+        <v>Minsk&amp;\bf{197}&amp;201.1&amp;PG&amp;238&amp;240.4\\</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -3555,15 +3548,15 @@
       <c r="K59" s="1"/>
       <c r="L59" s="1">
         <f t="shared" ref="L59" si="9">AVERAGE(L34:L58)</f>
-        <v>111.8</v>
+        <v>110.72</v>
       </c>
       <c r="M59" s="1">
         <f t="shared" ref="M59" si="10">AVERAGE(M34:M58)</f>
-        <v>113.44800000000001</v>
+        <v>112.40800000000002</v>
       </c>
       <c r="N59" s="1">
         <f t="shared" ref="N59" si="11">AVERAGE(N34:N58)</f>
-        <v>1.0880000000000001</v>
+        <v>1.0920000000000001</v>
       </c>
       <c r="P59" t="s">
         <v>75</v>
@@ -3571,31 +3564,31 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4" t="s">
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="7"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -4891,17 +4884,17 @@
         <v>48</v>
       </c>
       <c r="L87" s="2">
-        <v>317</v>
+        <v>388</v>
       </c>
       <c r="M87" s="2">
-        <v>318.5</v>
+        <v>390.2</v>
       </c>
       <c r="N87" s="2">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="P87" t="str">
         <f t="shared" si="13"/>
-        <v>Dublin&amp;363&amp;363&amp;PG&amp;\bf{317}&amp;318.5\\</v>
+        <v>Dublin&amp;\bf{363}&amp;363&amp;PG&amp;388&amp;390.2\\</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
@@ -4936,17 +4929,17 @@
         <v>48</v>
       </c>
       <c r="L88" s="2">
-        <v>506</v>
+        <v>454</v>
       </c>
       <c r="M88" s="2">
-        <v>509.4</v>
+        <v>457.6</v>
       </c>
       <c r="N88" s="2">
-        <v>2.9</v>
+        <v>2.4</v>
       </c>
       <c r="P88" t="str">
         <f t="shared" si="13"/>
-        <v>Minsk&amp;\bf{387}&amp;391.5&amp;PG&amp;506&amp;509.4\\</v>
+        <v>Minsk&amp;\bf{387}&amp;391.5&amp;PG&amp;454&amp;457.6\\</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
@@ -4992,11 +4985,11 @@
       <c r="K89" s="1"/>
       <c r="L89" s="1">
         <f t="shared" ref="L89" si="21">AVERAGE(L64:L88)</f>
-        <v>208.08</v>
+        <v>208.84</v>
       </c>
       <c r="M89" s="1">
         <f t="shared" ref="M89" si="22">AVERAGE(M64:M88)</f>
-        <v>210.06399999999996</v>
+        <v>210.86</v>
       </c>
       <c r="N89" s="1">
         <f t="shared" ref="N89" si="23">AVERAGE(N64:N88)</f>
@@ -5760,66 +5753,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="B1" s="5">
+      <c r="B1" s="8">
         <v>12345</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8">
         <v>22411</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8">
         <v>25233</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5">
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8">
         <v>52331</v>
       </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5">
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8">
         <v>54278</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5">
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8">
         <v>54433</v>
       </c>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5">
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8">
         <v>66655</v>
       </c>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5">
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8">
         <v>68531</v>
       </c>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5">
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8">
         <v>87744</v>
       </c>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5">
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8">
         <v>98811</v>
       </c>
-      <c r="AM1" s="5"/>
-      <c r="AN1" s="5"/>
-      <c r="AO1" s="5"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="8"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -9099,66 +9092,66 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="B1" s="5">
+      <c r="B1" s="8">
         <v>12345</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8">
         <v>22411</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8">
         <v>25233</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5">
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8">
         <v>52331</v>
       </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5">
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8">
         <v>54278</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5">
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8">
         <v>54433</v>
       </c>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5">
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8">
         <v>66655</v>
       </c>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5">
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8">
         <v>68531</v>
       </c>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5">
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8">
         <v>87744</v>
       </c>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5">
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8">
         <v>98811</v>
       </c>
-      <c r="AM1" s="5"/>
-      <c r="AN1" s="5"/>
-      <c r="AO1" s="5"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="8"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -12438,66 +12431,66 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="B1" s="5">
+      <c r="B1" s="8">
         <v>12345</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8">
         <v>22411</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8">
         <v>25233</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5">
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8">
         <v>52331</v>
       </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5">
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8">
         <v>54278</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5">
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8">
         <v>54433</v>
       </c>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5">
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8">
         <v>66655</v>
       </c>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5">
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8">
         <v>68531</v>
       </c>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5">
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8">
         <v>87744</v>
       </c>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5">
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8">
         <v>98811</v>
       </c>
-      <c r="AM1" s="5"/>
-      <c r="AN1" s="5"/>
-      <c r="AO1" s="5"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="8"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">

</xml_diff>